<commit_message>
Analysis update:     * Corrections to the Analysis sheet;     * Analysis of RBS2 and ERD detector added;     * SimNRA simulations added;
</commit_message>
<xml_diff>
--- a/Nat-Pb_Tests/032_RBS_21Janeiro/Logbook-RBS_21Janeiro.xlsx
+++ b/Nat-Pb_Tests/032_RBS_21Janeiro/Logbook-RBS_21Janeiro.xlsx
@@ -424,7 +424,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -623,6 +623,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFDEEBF7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFFBE5D6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFFFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFDAE3F3"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="32">
     <border>
@@ -1280,9 +1304,6 @@
     <xf numFmtId="2" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1307,9 +1328,6 @@
     <xf numFmtId="2" fontId="0" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1340,9 +1358,6 @@
     <xf numFmtId="2" fontId="0" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1353,9 +1368,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="25" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1389,9 +1401,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1621,6 +1630,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1941,11 +1965,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1988321616"/>
-        <c:axId val="1988325968"/>
+        <c:axId val="-208579264"/>
+        <c:axId val="-208575456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1988321616"/>
+        <c:axId val="-208579264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2023,12 +2047,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1988325968"/>
+        <c:crossAx val="-208575456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1988325968"/>
+        <c:axId val="-208575456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2106,7 +2130,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1988321616"/>
+        <c:crossAx val="-208579264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2244,10 +2268,10 @@
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>16.114908140961788</c:v>
+                    <c:v>16.190577449985792</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>48.344724422885328</c:v>
+                    <c:v>48.571732349957387</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2262,10 +2286,10 @@
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>16.114908140961788</c:v>
+                    <c:v>16.190577449985792</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>48.344724422885328</c:v>
+                    <c:v>48.571732349957387</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2349,11 +2373,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1988326512"/>
-        <c:axId val="1988327056"/>
+        <c:axId val="-208581984"/>
+        <c:axId val="-208584704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1988326512"/>
+        <c:axId val="-208581984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2434,12 +2458,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1988327056"/>
+        <c:crossAx val="-208584704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1988327056"/>
+        <c:axId val="-208584704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2557,7 +2581,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1988326512"/>
+        <c:crossAx val="-208581984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3705,7 +3729,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="212">
+      <c r="A7" s="207">
         <v>1</v>
       </c>
       <c r="B7" s="25">
@@ -3746,7 +3770,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="212">
+      <c r="A9" s="207">
         <v>1</v>
       </c>
       <c r="B9" s="26">
@@ -3783,7 +3807,7 @@
       <c r="H10" s="27"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="212">
+      <c r="A11" s="207">
         <v>1</v>
       </c>
       <c r="B11" s="27">
@@ -3828,7 +3852,7 @@
       <c r="L12" s="3"/>
     </row>
     <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="212">
+      <c r="A13" s="207">
         <v>1</v>
       </c>
       <c r="B13" s="47">
@@ -3915,7 +3939,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A17" s="212"/>
+      <c r="A17" s="207"/>
       <c r="B17" s="30">
         <v>13</v>
       </c>
@@ -3964,7 +3988,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="212"/>
+      <c r="A19" s="207"/>
       <c r="B19" s="32">
         <v>15</v>
       </c>
@@ -3997,7 +4021,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A21" s="212"/>
+      <c r="A21" s="207"/>
       <c r="B21" s="58">
         <v>17</v>
       </c>
@@ -4015,7 +4039,7 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="212"/>
+      <c r="A22" s="207"/>
       <c r="B22" s="62">
         <v>18</v>
       </c>
@@ -4054,7 +4078,7 @@
       </c>
     </row>
     <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="212"/>
+      <c r="A24" s="207"/>
       <c r="B24" s="69">
         <v>20</v>
       </c>
@@ -4092,8 +4116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="S12" sqref="S11:S12"/>
+    <sheetView tabSelected="1" topLeftCell="G30" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="Q37" sqref="Q37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4194,482 +4218,482 @@
         <f>$B$1*F4</f>
         <v>1563.7159776396684</v>
       </c>
-      <c r="H4" s="88">
+      <c r="H4" s="208">
         <v>643</v>
       </c>
       <c r="I4">
         <f>H4-'[1]Ta-Nb-V Calib - RBS1 - Alfa'!I2</f>
         <v>374</v>
       </c>
-      <c r="S4" s="89" t="s">
+      <c r="S4" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="T4" s="90"/>
-      <c r="U4" s="91" t="s">
+      <c r="T4" s="89"/>
+      <c r="U4" s="90" t="s">
         <v>45</v>
       </c>
-      <c r="V4" s="92"/>
-      <c r="W4" s="91"/>
-      <c r="X4" s="91" t="s">
+      <c r="V4" s="91"/>
+      <c r="W4" s="90"/>
+      <c r="X4" s="90" t="s">
         <v>46</v>
       </c>
-      <c r="Y4" s="92"/>
+      <c r="Y4" s="91"/>
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.35">
-      <c r="C5" s="93" t="s">
+      <c r="C5" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="94">
+      <c r="D5" s="93">
         <v>14</v>
       </c>
-      <c r="E5" s="95">
+      <c r="E5" s="94">
         <v>28.085000000000001</v>
       </c>
       <c r="F5" s="86">
         <f t="shared" si="0"/>
         <v>0.86930741306534087</v>
       </c>
-      <c r="G5" s="96">
+      <c r="G5" s="95">
         <f>$B$1*F5</f>
         <v>1738.6148261306816</v>
       </c>
-      <c r="H5" s="97">
+      <c r="H5" s="209">
         <v>712</v>
       </c>
       <c r="I5">
         <f>H5-'[1]Ta-Nb-V Calib - RBS1 - Alfa'!I3</f>
         <v>275</v>
       </c>
-      <c r="S5" s="98">
+      <c r="S5" s="96">
         <v>4</v>
       </c>
-      <c r="T5" s="99">
+      <c r="T5" s="97">
         <f>T13</f>
         <v>732.70189479750047</v>
       </c>
-      <c r="U5" s="100" t="s">
+      <c r="U5" s="98" t="s">
         <v>48</v>
       </c>
-      <c r="V5" s="101">
+      <c r="V5" s="99">
         <f>V13</f>
         <v>0</v>
       </c>
-      <c r="W5" s="102">
+      <c r="W5" s="100">
         <f>T5*344.092/0.30397*10^(-6)</f>
         <v>0.8294136276101638</v>
       </c>
-      <c r="X5" s="100" t="s">
+      <c r="X5" s="98" t="s">
         <v>48</v>
       </c>
-      <c r="Y5" s="103">
+      <c r="Y5" s="101">
         <f>V5*344.092/0.30397*10^(-6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.35">
-      <c r="C6" s="104" t="s">
+      <c r="C6" s="102" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="105">
+      <c r="D6" s="103">
         <v>23</v>
       </c>
-      <c r="E6" s="106">
+      <c r="E6" s="104">
         <v>50.942</v>
       </c>
       <c r="F6" s="86">
         <f t="shared" si="0"/>
         <v>0.9257111865667883</v>
       </c>
-      <c r="G6" s="107">
+      <c r="G6" s="105">
         <f>$B$1*F6</f>
         <v>1851.4223731335767</v>
       </c>
-      <c r="H6" s="108">
+      <c r="H6" s="210">
         <v>761</v>
       </c>
       <c r="I6">
         <f>H6-'[1]Ta-Nb-V Calib - RBS1 - Alfa'!I4</f>
         <v>179</v>
       </c>
-      <c r="S6" s="98">
+      <c r="S6" s="96">
         <v>5</v>
       </c>
-      <c r="T6" s="99">
+      <c r="T6" s="97">
         <f>T18</f>
-        <v>512.77323711025656</v>
-      </c>
-      <c r="U6" s="100" t="s">
+        <v>515.18101977949254</v>
+      </c>
+      <c r="U6" s="98" t="s">
         <v>48</v>
       </c>
-      <c r="V6" s="101">
+      <c r="V6" s="99">
         <f>V18</f>
-        <v>16.114908140961788</v>
-      </c>
-      <c r="W6" s="102">
+        <v>16.190577449985792</v>
+      </c>
+      <c r="W6" s="100">
         <f t="shared" ref="W6:W7" si="1">T6*344.092/0.30397*10^(-6)</f>
-        <v>0.58045586309090491</v>
-      </c>
-      <c r="X6" s="100" t="s">
+        <v>0.58318145691339651</v>
+      </c>
+      <c r="X6" s="98" t="s">
         <v>48</v>
       </c>
-      <c r="Y6" s="103">
+      <c r="Y6" s="101">
         <f t="shared" ref="Y6:Y7" si="2">V6*344.092/0.30397*10^(-6)</f>
-        <v>1.8241967865380869E-2</v>
+        <v>1.8327625015365039E-2</v>
       </c>
     </row>
     <row r="7" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C7" s="109" t="s">
+      <c r="C7" s="106" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="110">
+      <c r="D7" s="107">
         <v>41</v>
       </c>
-      <c r="E7" s="111">
+      <c r="E7" s="108">
         <v>92.906000000000006</v>
       </c>
       <c r="F7" s="86">
         <f t="shared" si="0"/>
         <v>0.95856067934676659</v>
       </c>
-      <c r="G7" s="112">
+      <c r="G7" s="109">
         <f>$B$1*F7</f>
         <v>1917.1213586935332</v>
       </c>
-      <c r="H7" s="113">
+      <c r="H7" s="211">
         <v>792</v>
       </c>
       <c r="I7">
         <f>H7-'[1]Ta-Nb-V Calib - RBS1 - Alfa'!I5</f>
         <v>119</v>
       </c>
-      <c r="S7" s="114">
+      <c r="S7" s="110">
         <v>6</v>
       </c>
-      <c r="T7" s="115">
+      <c r="T7" s="111">
         <f>T23</f>
-        <v>968.57167009715113</v>
-      </c>
-      <c r="U7" s="116" t="s">
+        <v>973.11970402793031</v>
+      </c>
+      <c r="U7" s="112" t="s">
         <v>48</v>
       </c>
-      <c r="V7" s="117">
+      <c r="V7" s="113">
         <f>V23</f>
-        <v>48.344724422885328</v>
-      </c>
-      <c r="W7" s="118">
+        <v>48.571732349957387</v>
+      </c>
+      <c r="W7" s="114">
         <f t="shared" si="1"/>
-        <v>1.0964166302828202</v>
-      </c>
-      <c r="X7" s="116" t="s">
+        <v>1.1015649741697489</v>
+      </c>
+      <c r="X7" s="112" t="s">
         <v>48</v>
       </c>
-      <c r="Y7" s="119">
+      <c r="Y7" s="115">
         <f t="shared" si="2"/>
-        <v>5.4725903596142565E-2</v>
+        <v>5.4982875046095114E-2</v>
       </c>
     </row>
     <row r="8" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C8" s="120" t="s">
+      <c r="C8" s="116" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="121">
+      <c r="D8" s="117">
         <v>73</v>
       </c>
-      <c r="E8" s="122">
+      <c r="E8" s="118">
         <v>180.95</v>
       </c>
-      <c r="F8" s="123">
+      <c r="F8" s="119">
         <f t="shared" si="0"/>
         <v>0.97850521298958393</v>
       </c>
-      <c r="G8" s="124">
+      <c r="G8" s="120">
         <f>$B$1*F8</f>
         <v>1957.0104259791678</v>
       </c>
-      <c r="H8" s="125">
+      <c r="H8" s="212">
         <v>808</v>
       </c>
-      <c r="I8" s="202">
+      <c r="I8" s="197">
         <f>H8-'[1]Ta-Nb-V Calib - RBS1 - Alfa'!I6</f>
         <v>75.5</v>
       </c>
-      <c r="J8" s="126"/>
-      <c r="S8" s="114">
+      <c r="J8" s="121"/>
+      <c r="S8" s="110">
         <v>7</v>
       </c>
-      <c r="T8" s="115">
+      <c r="T8" s="111">
         <f>T24</f>
         <v>0</v>
       </c>
-      <c r="U8" s="116" t="s">
+      <c r="U8" s="112" t="s">
         <v>48</v>
       </c>
-      <c r="V8" s="117">
+      <c r="V8" s="113">
         <f>V24</f>
         <v>0</v>
       </c>
-      <c r="W8" s="118">
+      <c r="W8" s="114">
         <f t="shared" ref="W8" si="3">T8*344.092/0.30397*10^(-6)</f>
         <v>0</v>
       </c>
-      <c r="X8" s="116" t="s">
+      <c r="X8" s="112" t="s">
         <v>48</v>
       </c>
-      <c r="Y8" s="119">
+      <c r="Y8" s="115">
         <f t="shared" ref="Y8" si="4">V8*344.092/0.30397*10^(-6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C9" s="127" t="s">
+      <c r="C9" s="122" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="128">
+      <c r="D9" s="123">
         <v>82</v>
       </c>
-      <c r="E9" s="128">
+      <c r="E9" s="123">
         <v>207.2</v>
       </c>
-      <c r="F9" s="129">
+      <c r="F9" s="124">
         <f t="shared" si="0"/>
         <v>0.9812026480871997</v>
       </c>
-      <c r="G9" s="130">
+      <c r="G9" s="125">
         <f t="shared" ref="G9:G12" si="5">$B$1*F9</f>
         <v>1962.4052961743994</v>
       </c>
-      <c r="H9" s="131">
+      <c r="H9" s="126">
         <f>(G9-46.367)/2.3671</f>
         <v>809.4454379512481</v>
       </c>
-      <c r="I9" s="202">
+      <c r="I9" s="197">
         <f>H9-'[1]Ta-Nb-V Calib - RBS1 - Alfa'!I7</f>
         <v>66.496141609777283</v>
       </c>
     </row>
     <row r="10" spans="1:48" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="J10" s="2"/>
-      <c r="K10" s="132" t="s">
+      <c r="K10" s="127" t="s">
         <v>68</v>
       </c>
-      <c r="L10" s="133" t="s">
+      <c r="L10" s="128" t="s">
         <v>54</v>
       </c>
-      <c r="M10" s="134" t="s">
+      <c r="M10" s="129" t="s">
         <v>55</v>
       </c>
-      <c r="N10" s="135" t="s">
+      <c r="N10" s="130" t="s">
         <v>56</v>
       </c>
-      <c r="O10" s="134" t="s">
+      <c r="O10" s="129" t="s">
         <v>57</v>
       </c>
-      <c r="P10" s="135" t="s">
+      <c r="P10" s="130" t="s">
         <v>58</v>
       </c>
-      <c r="Q10" s="134" t="s">
+      <c r="Q10" s="129" t="s">
         <v>59</v>
       </c>
-      <c r="R10" s="135" t="s">
+      <c r="R10" s="130" t="s">
         <v>60</v>
       </c>
-      <c r="S10" s="136" t="s">
+      <c r="S10" s="131" t="s">
         <v>61</v>
       </c>
-      <c r="T10" s="137" t="s">
+      <c r="T10" s="132" t="s">
         <v>62</v>
       </c>
-      <c r="U10" s="138"/>
-      <c r="V10" s="139"/>
-      <c r="X10" s="186"/>
-      <c r="Y10" s="187" t="s">
+      <c r="U10" s="133"/>
+      <c r="V10" s="134"/>
+      <c r="X10" s="181"/>
+      <c r="Y10" s="182" t="s">
         <v>65</v>
       </c>
-      <c r="Z10" s="188" t="s">
+      <c r="Z10" s="183" t="s">
         <v>66</v>
       </c>
-      <c r="AA10" s="188" t="s">
+      <c r="AA10" s="183" t="s">
         <v>56</v>
       </c>
-      <c r="AB10" s="188" t="s">
+      <c r="AB10" s="183" t="s">
         <v>57</v>
       </c>
-      <c r="AC10" s="188" t="s">
+      <c r="AC10" s="183" t="s">
         <v>58</v>
       </c>
-      <c r="AD10" s="188" t="s">
+      <c r="AD10" s="183" t="s">
         <v>59</v>
       </c>
-      <c r="AE10" s="188" t="s">
+      <c r="AE10" s="183" t="s">
         <v>60</v>
       </c>
-      <c r="AF10" s="189" t="s">
+      <c r="AF10" s="184" t="s">
         <v>61</v>
       </c>
-      <c r="AG10" s="190" t="s">
+      <c r="AG10" s="185" t="s">
         <v>62</v>
       </c>
-      <c r="AH10" s="138"/>
-      <c r="AI10" s="139"/>
-      <c r="AK10" s="140"/>
-      <c r="AL10" s="141" t="s">
+      <c r="AH10" s="133"/>
+      <c r="AI10" s="134"/>
+      <c r="AK10" s="135"/>
+      <c r="AL10" s="136" t="s">
         <v>63</v>
       </c>
-      <c r="AM10" s="142" t="s">
+      <c r="AM10" s="137" t="s">
         <v>64</v>
       </c>
-      <c r="AN10" s="142" t="s">
+      <c r="AN10" s="137" t="s">
         <v>56</v>
       </c>
-      <c r="AO10" s="142" t="s">
+      <c r="AO10" s="137" t="s">
         <v>57</v>
       </c>
-      <c r="AP10" s="142" t="s">
+      <c r="AP10" s="137" t="s">
         <v>58</v>
       </c>
-      <c r="AQ10" s="142" t="s">
+      <c r="AQ10" s="137" t="s">
         <v>59</v>
       </c>
-      <c r="AR10" s="142" t="s">
+      <c r="AR10" s="137" t="s">
         <v>60</v>
       </c>
-      <c r="AS10" s="143" t="s">
+      <c r="AS10" s="138" t="s">
         <v>61</v>
       </c>
-      <c r="AT10" s="144" t="s">
+      <c r="AT10" s="139" t="s">
         <v>62</v>
       </c>
-      <c r="AU10" s="138"/>
-      <c r="AV10" s="139"/>
+      <c r="AU10" s="133"/>
+      <c r="AV10" s="134"/>
     </row>
     <row r="11" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C11" s="206" t="s">
+      <c r="C11" s="201" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="207">
+      <c r="D11" s="202">
         <v>17</v>
       </c>
-      <c r="E11" s="207">
+      <c r="E11" s="202">
         <v>35.450000000000003</v>
       </c>
-      <c r="F11" s="204">
+      <c r="F11" s="199">
         <f t="shared" si="0"/>
         <v>0.89499019427127813</v>
       </c>
-      <c r="G11" s="205">
+      <c r="G11" s="200">
         <f t="shared" si="5"/>
         <v>1789.9803885425563</v>
       </c>
-      <c r="H11" s="208">
+      <c r="H11" s="203">
         <f>(G11-46.367)/2.3671</f>
         <v>736.60318049197588</v>
       </c>
-      <c r="K11" s="145" t="s">
+      <c r="K11" s="140" t="s">
         <v>69</v>
       </c>
-      <c r="L11" s="146">
+      <c r="L11" s="141">
         <v>808</v>
       </c>
-      <c r="M11" s="147">
+      <c r="M11" s="142">
         <v>776</v>
       </c>
-      <c r="N11" s="148">
+      <c r="N11" s="143">
         <f>(L11-M11)*2.381</f>
         <v>76.191999999999993</v>
       </c>
-      <c r="O11" s="147">
+      <c r="O11" s="142">
         <v>45.37</v>
       </c>
-      <c r="P11" s="149">
+      <c r="P11" s="144">
         <f>O11*$B$2/10</f>
         <v>51.313469999999995</v>
       </c>
-      <c r="Q11" s="147">
+      <c r="Q11" s="142">
         <v>45.81</v>
       </c>
-      <c r="R11" s="150">
+      <c r="R11" s="145">
         <f>Q11*$B$2/10</f>
         <v>51.811110000000006</v>
       </c>
-      <c r="S11" s="151">
+      <c r="S11" s="146">
         <f t="shared" ref="S11:S12" si="6">(($F$9/COS(RADIANS(0))*P11)+(1/COS(RADIANS(15))*R11))</f>
         <v>103.98772071014974</v>
       </c>
-      <c r="T11" s="152">
+      <c r="T11" s="147">
         <f>N11*10^3/S11</f>
         <v>732.70189479750047</v>
       </c>
-      <c r="U11" s="153"/>
-      <c r="V11" s="154">
+      <c r="U11" s="148"/>
+      <c r="V11" s="149">
         <f>($T$13-T11)^2</f>
         <v>0</v>
       </c>
-      <c r="X11" s="191"/>
-      <c r="Y11" s="146">
+      <c r="X11" s="186"/>
+      <c r="Y11" s="141">
         <v>612</v>
       </c>
-      <c r="Z11" s="147"/>
-      <c r="AA11" s="148">
+      <c r="Z11" s="142"/>
+      <c r="AA11" s="143">
         <f>(Y11-Z11)*2.381</f>
         <v>1457.1719999999998</v>
       </c>
-      <c r="AB11" s="147">
+      <c r="AB11" s="142">
         <v>133.5</v>
       </c>
-      <c r="AC11" s="149">
+      <c r="AC11" s="144">
         <f>AB11*$B$2/10</f>
         <v>150.98849999999999</v>
       </c>
-      <c r="AD11" s="147">
+      <c r="AD11" s="142">
         <v>135.30000000000001</v>
       </c>
-      <c r="AE11" s="150">
+      <c r="AE11" s="145">
         <f>AD11*$B$2/10</f>
         <v>153.02430000000001</v>
       </c>
-      <c r="AF11" s="151">
+      <c r="AF11" s="146">
         <f>(($F$9/COS(RADIANS(0))*AC11)+(1/COS(RADIANS(15)*AE11)))</f>
         <v>146.74501411526421</v>
       </c>
-      <c r="AG11" s="197">
+      <c r="AG11" s="192">
         <f>AA11*10^3/AF11</f>
         <v>9929.9591797744542</v>
       </c>
-      <c r="AH11" s="153"/>
-      <c r="AI11" s="156"/>
-      <c r="AK11" s="155"/>
-      <c r="AL11" s="146">
+      <c r="AH11" s="148"/>
+      <c r="AI11" s="151"/>
+      <c r="AK11" s="150"/>
+      <c r="AL11" s="141">
         <v>560</v>
       </c>
-      <c r="AM11" s="147"/>
-      <c r="AN11" s="148">
+      <c r="AM11" s="142"/>
+      <c r="AN11" s="143">
         <f>(AL11-AM11)*2.381</f>
         <v>1333.36</v>
       </c>
-      <c r="AO11" s="147">
+      <c r="AO11" s="142">
         <v>139.5</v>
       </c>
-      <c r="AP11" s="149">
+      <c r="AP11" s="144">
         <f>AO11*$B$2/10</f>
         <v>157.77450000000002</v>
       </c>
-      <c r="AQ11" s="147">
+      <c r="AQ11" s="142">
         <v>141.5</v>
       </c>
-      <c r="AR11" s="150">
+      <c r="AR11" s="145">
         <f>AQ11*$B$2/10</f>
         <v>160.03649999999999</v>
       </c>
-      <c r="AS11" s="151">
+      <c r="AS11" s="146">
         <f>(($F$9/COS(RADIANS(0))*AP11)+(1/COS(RADIANS(15)*AR11)))</f>
         <v>152.7750043830697</v>
       </c>
-      <c r="AT11" s="197">
+      <c r="AT11" s="192">
         <f>AN11*10^3/AS11</f>
         <v>8727.605706079501</v>
       </c>
-      <c r="AU11" s="153"/>
-      <c r="AV11" s="156"/>
+      <c r="AU11" s="148"/>
+      <c r="AV11" s="151"/>
     </row>
     <row r="12" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" t="s">
@@ -4681,147 +4705,147 @@
       <c r="E12">
         <v>63.545999999999999</v>
       </c>
-      <c r="F12" s="204">
+      <c r="F12" s="199">
         <f t="shared" si="0"/>
         <v>0.93999634329545045</v>
       </c>
-      <c r="G12" s="205">
+      <c r="G12" s="200">
         <f t="shared" si="5"/>
         <v>1879.9926865909008</v>
       </c>
-      <c r="H12" s="208">
+      <c r="H12" s="203">
         <f>(G12-46.367)/2.3671</f>
         <v>774.62958328372304</v>
       </c>
-      <c r="K12" s="162" t="s">
+      <c r="K12" s="157" t="s">
         <v>70</v>
       </c>
-      <c r="L12" s="163">
+      <c r="L12" s="158">
         <v>808</v>
       </c>
-      <c r="M12" s="164">
+      <c r="M12" s="159">
         <v>776</v>
       </c>
-      <c r="N12" s="165">
+      <c r="N12" s="160">
         <f t="shared" ref="N12" si="7">(L12-M12)*2.381</f>
         <v>76.191999999999993</v>
       </c>
-      <c r="O12" s="166">
+      <c r="O12" s="161">
         <v>45.37</v>
       </c>
-      <c r="P12" s="167">
+      <c r="P12" s="162">
         <f t="shared" ref="P12" si="8">O12*$B$2/10</f>
         <v>51.313469999999995</v>
       </c>
-      <c r="Q12" s="166">
+      <c r="Q12" s="161">
         <v>45.81</v>
       </c>
-      <c r="R12" s="168">
+      <c r="R12" s="163">
         <f t="shared" ref="R12" si="9">Q12*$B$2/10</f>
         <v>51.811110000000006</v>
       </c>
-      <c r="S12" s="151">
+      <c r="S12" s="146">
         <f t="shared" si="6"/>
         <v>103.98772071014974</v>
       </c>
-      <c r="T12" s="170">
+      <c r="T12" s="165">
         <f>N12*10^3/S12</f>
         <v>732.70189479750047</v>
       </c>
-      <c r="U12" s="153"/>
-      <c r="V12" s="154">
+      <c r="U12" s="148"/>
+      <c r="V12" s="149">
         <f>($T$13-T12)^2</f>
         <v>0</v>
       </c>
-      <c r="X12" s="192"/>
-      <c r="Y12" s="157">
+      <c r="X12" s="187"/>
+      <c r="Y12" s="152">
         <v>611</v>
       </c>
-      <c r="Z12" s="158"/>
-      <c r="AA12" s="148">
+      <c r="Z12" s="153"/>
+      <c r="AA12" s="143">
         <f>(Y12-Z12)*2.381</f>
         <v>1454.7909999999999</v>
       </c>
-      <c r="AB12" s="147">
+      <c r="AB12" s="142">
         <v>133.5</v>
       </c>
-      <c r="AC12" s="159">
+      <c r="AC12" s="154">
         <f t="shared" ref="AC12" si="10">AB12*$B$2/10</f>
         <v>150.98849999999999</v>
       </c>
-      <c r="AD12" s="147">
+      <c r="AD12" s="142">
         <v>135.30000000000001</v>
       </c>
-      <c r="AE12" s="160">
+      <c r="AE12" s="155">
         <f t="shared" ref="AE12" si="11">AD12*$B$2/10</f>
         <v>153.02430000000001</v>
       </c>
-      <c r="AF12" s="151">
+      <c r="AF12" s="146">
         <f t="shared" ref="AF12" si="12">(($F$9/COS(RADIANS(0))*AC12)+(1/COS(RADIANS(15)*AE12)))</f>
         <v>146.74501411526421</v>
       </c>
-      <c r="AG12" s="198">
+      <c r="AG12" s="193">
         <f>AA12*10^3/AF12</f>
         <v>9913.7337562780922</v>
       </c>
-      <c r="AH12" s="153"/>
-      <c r="AI12" s="156"/>
-      <c r="AK12" s="161"/>
-      <c r="AL12" s="157">
+      <c r="AH12" s="148"/>
+      <c r="AI12" s="151"/>
+      <c r="AK12" s="156"/>
+      <c r="AL12" s="152">
         <v>560</v>
       </c>
-      <c r="AM12" s="158"/>
-      <c r="AN12" s="148">
+      <c r="AM12" s="153"/>
+      <c r="AN12" s="143">
         <f t="shared" ref="AN12" si="13">(AL12-AM12)*2.381</f>
         <v>1333.36</v>
       </c>
-      <c r="AO12" s="147">
+      <c r="AO12" s="142">
         <v>139.5</v>
       </c>
-      <c r="AP12" s="159">
+      <c r="AP12" s="154">
         <f t="shared" ref="AP12" si="14">AO12*$B$2/10</f>
         <v>157.77450000000002</v>
       </c>
-      <c r="AQ12" s="147">
+      <c r="AQ12" s="142">
         <v>141.5</v>
       </c>
-      <c r="AR12" s="160">
+      <c r="AR12" s="155">
         <f t="shared" ref="AR12" si="15">AQ12*$B$2/10</f>
         <v>160.03649999999999</v>
       </c>
-      <c r="AS12" s="151">
+      <c r="AS12" s="146">
         <f>(($F$9/COS(RADIANS(0))*AP12)+(1/COS(RADIANS(15)*AR12)))</f>
         <v>152.7750043830697</v>
       </c>
-      <c r="AT12" s="198">
+      <c r="AT12" s="193">
         <f>AN12*10^3/AS12</f>
         <v>8727.605706079501</v>
       </c>
-      <c r="AU12" s="153"/>
-      <c r="AV12" s="156"/>
+      <c r="AU12" s="148"/>
+      <c r="AV12" s="151"/>
     </row>
     <row r="13" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K13" s="172"/>
-      <c r="L13" s="153"/>
-      <c r="M13" s="153"/>
-      <c r="N13" s="153"/>
-      <c r="O13" s="153"/>
-      <c r="P13" s="153"/>
-      <c r="Q13" s="153"/>
-      <c r="R13" s="153"/>
-      <c r="S13" s="153"/>
-      <c r="T13" s="173">
+      <c r="K13" s="167"/>
+      <c r="L13" s="148"/>
+      <c r="M13" s="148"/>
+      <c r="N13" s="148"/>
+      <c r="O13" s="148"/>
+      <c r="P13" s="148"/>
+      <c r="Q13" s="148"/>
+      <c r="R13" s="148"/>
+      <c r="S13" s="148"/>
+      <c r="T13" s="168">
         <f>SUM(T11:T12)/2</f>
         <v>732.70189479750047</v>
       </c>
-      <c r="U13" s="174" t="s">
+      <c r="U13" s="169" t="s">
         <v>48</v>
       </c>
-      <c r="V13" s="175">
+      <c r="V13" s="170">
         <f>SQRT(SUM(V11:V12))</f>
         <v>0</v>
       </c>
-      <c r="X13" s="176"/>
+      <c r="X13" s="171"/>
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
       <c r="AA13" s="3"/>
@@ -4831,9 +4855,9 @@
       <c r="AE13" s="3"/>
       <c r="AF13" s="3"/>
       <c r="AG13" s="3"/>
-      <c r="AH13" s="153"/>
-      <c r="AI13" s="156"/>
-      <c r="AK13" s="176"/>
+      <c r="AH13" s="148"/>
+      <c r="AI13" s="151"/>
+      <c r="AK13" s="171"/>
       <c r="AL13" s="3"/>
       <c r="AM13" s="3"/>
       <c r="AN13" s="3"/>
@@ -4842,24 +4866,24 @@
       <c r="AQ13" s="3"/>
       <c r="AR13" s="3"/>
       <c r="AS13" s="3"/>
-      <c r="AT13" s="200"/>
-      <c r="AU13" s="153"/>
-      <c r="AV13" s="156"/>
+      <c r="AT13" s="195"/>
+      <c r="AU13" s="148"/>
+      <c r="AV13" s="151"/>
     </row>
     <row r="14" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K14" s="172"/>
-      <c r="L14" s="153"/>
-      <c r="M14" s="153"/>
-      <c r="N14" s="153"/>
-      <c r="O14" s="153"/>
-      <c r="P14" s="153"/>
-      <c r="Q14" s="153"/>
-      <c r="R14" s="153"/>
-      <c r="S14" s="153"/>
-      <c r="T14" s="153"/>
-      <c r="U14" s="153"/>
-      <c r="V14" s="156"/>
-      <c r="X14" s="176"/>
+      <c r="K14" s="167"/>
+      <c r="L14" s="148"/>
+      <c r="M14" s="148"/>
+      <c r="N14" s="148"/>
+      <c r="O14" s="148"/>
+      <c r="P14" s="148"/>
+      <c r="Q14" s="148"/>
+      <c r="R14" s="148"/>
+      <c r="S14" s="148"/>
+      <c r="T14" s="148"/>
+      <c r="U14" s="148"/>
+      <c r="V14" s="151"/>
+      <c r="X14" s="171"/>
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
       <c r="AA14" s="3"/>
@@ -4869,9 +4893,9 @@
       <c r="AE14" s="3"/>
       <c r="AF14" s="3"/>
       <c r="AG14" s="3"/>
-      <c r="AH14" s="153"/>
-      <c r="AI14" s="156"/>
-      <c r="AK14" s="176"/>
+      <c r="AH14" s="148"/>
+      <c r="AI14" s="151"/>
+      <c r="AK14" s="171"/>
       <c r="AL14" s="3"/>
       <c r="AM14" s="3"/>
       <c r="AN14" s="3"/>
@@ -4880,346 +4904,346 @@
       <c r="AQ14" s="3"/>
       <c r="AR14" s="3"/>
       <c r="AS14" s="3"/>
-      <c r="AT14" s="200"/>
-      <c r="AU14" s="153"/>
-      <c r="AV14" s="156"/>
+      <c r="AT14" s="195"/>
+      <c r="AU14" s="148"/>
+      <c r="AV14" s="151"/>
     </row>
     <row r="15" spans="1:48" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K15" s="132" t="s">
+      <c r="K15" s="127" t="s">
         <v>71</v>
       </c>
-      <c r="L15" s="133" t="s">
+      <c r="L15" s="128" t="s">
         <v>54</v>
       </c>
-      <c r="M15" s="134" t="s">
+      <c r="M15" s="129" t="s">
         <v>55</v>
       </c>
-      <c r="N15" s="135" t="s">
+      <c r="N15" s="130" t="s">
         <v>56</v>
       </c>
-      <c r="O15" s="134" t="s">
+      <c r="O15" s="129" t="s">
         <v>57</v>
       </c>
-      <c r="P15" s="135" t="s">
+      <c r="P15" s="130" t="s">
         <v>58</v>
       </c>
-      <c r="Q15" s="134" t="s">
+      <c r="Q15" s="129" t="s">
         <v>59</v>
       </c>
-      <c r="R15" s="135" t="s">
+      <c r="R15" s="130" t="s">
         <v>60</v>
       </c>
-      <c r="S15" s="136" t="s">
+      <c r="S15" s="131" t="s">
         <v>61</v>
       </c>
-      <c r="T15" s="137" t="s">
+      <c r="T15" s="132" t="s">
         <v>62</v>
       </c>
-      <c r="U15" s="153"/>
-      <c r="V15" s="156"/>
-      <c r="X15" s="186"/>
-      <c r="Y15" s="187" t="s">
+      <c r="U15" s="148"/>
+      <c r="V15" s="151"/>
+      <c r="X15" s="181"/>
+      <c r="Y15" s="182" t="s">
         <v>65</v>
       </c>
-      <c r="Z15" s="188" t="s">
+      <c r="Z15" s="183" t="s">
         <v>66</v>
       </c>
-      <c r="AA15" s="188" t="s">
+      <c r="AA15" s="183" t="s">
         <v>56</v>
       </c>
-      <c r="AB15" s="188" t="s">
+      <c r="AB15" s="183" t="s">
         <v>57</v>
       </c>
-      <c r="AC15" s="188" t="s">
+      <c r="AC15" s="183" t="s">
         <v>58</v>
       </c>
-      <c r="AD15" s="188" t="s">
+      <c r="AD15" s="183" t="s">
         <v>59</v>
       </c>
-      <c r="AE15" s="188" t="s">
+      <c r="AE15" s="183" t="s">
         <v>60</v>
       </c>
-      <c r="AF15" s="189" t="s">
+      <c r="AF15" s="184" t="s">
         <v>61</v>
       </c>
-      <c r="AG15" s="190" t="s">
+      <c r="AG15" s="185" t="s">
         <v>62</v>
       </c>
-      <c r="AH15" s="153"/>
-      <c r="AI15" s="156"/>
-      <c r="AK15" s="140"/>
-      <c r="AL15" s="141" t="s">
+      <c r="AH15" s="148"/>
+      <c r="AI15" s="151"/>
+      <c r="AK15" s="135"/>
+      <c r="AL15" s="136" t="s">
         <v>63</v>
       </c>
-      <c r="AM15" s="142" t="s">
+      <c r="AM15" s="137" t="s">
         <v>64</v>
       </c>
-      <c r="AN15" s="142" t="s">
+      <c r="AN15" s="137" t="s">
         <v>56</v>
       </c>
-      <c r="AO15" s="142" t="s">
+      <c r="AO15" s="137" t="s">
         <v>57</v>
       </c>
-      <c r="AP15" s="142" t="s">
+      <c r="AP15" s="137" t="s">
         <v>58</v>
       </c>
-      <c r="AQ15" s="142" t="s">
+      <c r="AQ15" s="137" t="s">
         <v>59</v>
       </c>
-      <c r="AR15" s="142" t="s">
+      <c r="AR15" s="137" t="s">
         <v>60</v>
       </c>
-      <c r="AS15" s="143" t="s">
+      <c r="AS15" s="138" t="s">
         <v>61</v>
       </c>
-      <c r="AT15" s="201" t="s">
+      <c r="AT15" s="196" t="s">
         <v>62</v>
       </c>
-      <c r="AU15" s="153"/>
-      <c r="AV15" s="156"/>
+      <c r="AU15" s="148"/>
+      <c r="AV15" s="151"/>
     </row>
     <row r="16" spans="1:48" x14ac:dyDescent="0.35">
-      <c r="K16" s="145" t="s">
+      <c r="K16" s="140" t="s">
         <v>72</v>
       </c>
-      <c r="L16" s="146">
+      <c r="L16" s="141">
         <v>811</v>
       </c>
-      <c r="M16" s="147">
+      <c r="M16" s="142">
         <v>789</v>
       </c>
-      <c r="N16" s="148">
+      <c r="N16" s="143">
         <f>(L16-M16)*2.381</f>
         <v>52.381999999999998</v>
       </c>
-      <c r="O16" s="147">
+      <c r="O16" s="142">
+        <v>45.37</v>
+      </c>
+      <c r="P16" s="142">
+        <f>O16*$B$2/10</f>
+        <v>51.313469999999995</v>
+      </c>
+      <c r="Q16" s="142">
         <v>45.81</v>
       </c>
-      <c r="P16" s="147">
-        <f>O16*$B$2/10</f>
-        <v>51.811110000000006</v>
-      </c>
-      <c r="Q16" s="147">
-        <v>45.81</v>
-      </c>
-      <c r="R16" s="147">
+      <c r="R16" s="142">
         <f>Q16*$B$2/10</f>
         <v>51.811110000000006</v>
       </c>
-      <c r="S16" s="151">
+      <c r="S16" s="146">
         <f t="shared" ref="S16:S17" si="16">(($F$9/COS(RADIANS(0))*P16)+(1/COS(RADIANS(15))*R16))</f>
-        <v>104.47600639594387</v>
-      </c>
-      <c r="T16" s="152">
+        <v>103.98772071014974</v>
+      </c>
+      <c r="T16" s="147">
         <f>N16*10^3/S16</f>
-        <v>501.37827628558415</v>
-      </c>
-      <c r="U16" s="153"/>
-      <c r="V16" s="154">
+        <v>503.73255267328159</v>
+      </c>
+      <c r="U16" s="148"/>
+      <c r="V16" s="149">
         <f>($T$18-T16)^2</f>
-        <v>129.84513219581893</v>
-      </c>
-      <c r="X16" s="191"/>
-      <c r="Y16" s="146">
+        <v>131.06739908199424</v>
+      </c>
+      <c r="X16" s="186"/>
+      <c r="Y16" s="141">
         <v>623</v>
       </c>
-      <c r="Z16" s="147"/>
-      <c r="AA16" s="148">
+      <c r="Z16" s="142"/>
+      <c r="AA16" s="143">
         <f t="shared" ref="AA16:AA17" si="17">(Y16-Z16)*2.381</f>
         <v>1483.3629999999998</v>
       </c>
-      <c r="AB16" s="147">
+      <c r="AB16" s="142">
         <v>133.5</v>
       </c>
-      <c r="AC16" s="147">
+      <c r="AC16" s="142">
         <f>AB16*$B$2/10</f>
         <v>150.98849999999999</v>
       </c>
-      <c r="AD16" s="147">
+      <c r="AD16" s="142">
         <v>135.30000000000001</v>
       </c>
-      <c r="AE16" s="147">
+      <c r="AE16" s="142">
         <f>AD16*$B$2/10</f>
         <v>153.02430000000001</v>
       </c>
-      <c r="AF16" s="151">
+      <c r="AF16" s="146">
         <f>(($F$9/COS(RADIANS(0))*AC16)+(1/COS(RADIANS(15)*AE16)))</f>
         <v>146.74501411526421</v>
       </c>
-      <c r="AG16" s="197">
+      <c r="AG16" s="192">
         <f>AA16*10^3/AF16</f>
         <v>10108.438838234453</v>
       </c>
-      <c r="AH16" s="153"/>
-      <c r="AI16" s="156"/>
-      <c r="AK16" s="155"/>
-      <c r="AL16" s="146">
+      <c r="AH16" s="148"/>
+      <c r="AI16" s="151"/>
+      <c r="AK16" s="150"/>
+      <c r="AL16" s="141">
         <v>571</v>
       </c>
-      <c r="AM16" s="147" t="s">
+      <c r="AM16" s="142" t="s">
         <v>73</v>
       </c>
-      <c r="AN16" s="148" t="e">
+      <c r="AN16" s="143" t="e">
         <f t="shared" ref="AN16:AN17" si="18">(AL16-AM16)*2.381</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AO16" s="147">
+      <c r="AO16" s="142">
         <v>139.5</v>
       </c>
-      <c r="AP16" s="147">
+      <c r="AP16" s="142">
         <f>AO16*$B$2/10</f>
         <v>157.77450000000002</v>
       </c>
-      <c r="AQ16" s="147">
+      <c r="AQ16" s="142">
         <v>141.5</v>
       </c>
-      <c r="AR16" s="147">
+      <c r="AR16" s="142">
         <f>AQ16*$B$2/10</f>
         <v>160.03649999999999</v>
       </c>
-      <c r="AS16" s="151">
+      <c r="AS16" s="146">
         <f>(($F$9/COS(RADIANS(0))*AP16)+(1/COS(RADIANS(15)*AR16)))</f>
         <v>152.7750043830697</v>
       </c>
-      <c r="AT16" s="197" t="e">
+      <c r="AT16" s="192" t="e">
         <f>AN16*10^3/AS16</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AU16" s="153"/>
-      <c r="AV16" s="156"/>
+      <c r="AU16" s="148"/>
+      <c r="AV16" s="151"/>
     </row>
     <row r="17" spans="11:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K17" s="162" t="s">
+      <c r="K17" s="157" t="s">
         <v>89</v>
       </c>
-      <c r="L17" s="177">
+      <c r="L17" s="172">
         <v>809</v>
       </c>
-      <c r="M17" s="178">
+      <c r="M17" s="173">
         <v>786</v>
       </c>
-      <c r="N17" s="165">
+      <c r="N17" s="160">
         <f>(L17-M17)*2.381</f>
         <v>54.762999999999998</v>
       </c>
-      <c r="O17" s="166">
+      <c r="O17" s="161">
+        <v>45.37</v>
+      </c>
+      <c r="P17" s="159">
+        <f t="shared" ref="P17" si="19">O17*$B$2/10</f>
+        <v>51.313469999999995</v>
+      </c>
+      <c r="Q17" s="161">
         <v>45.81</v>
       </c>
-      <c r="P17" s="164">
-        <f t="shared" ref="P17" si="19">O17*$B$2/10</f>
-        <v>51.811110000000006</v>
-      </c>
-      <c r="Q17" s="166">
-        <v>45.81</v>
-      </c>
-      <c r="R17" s="164">
+      <c r="R17" s="159">
         <f t="shared" ref="R17" si="20">Q17*$B$2/10</f>
         <v>51.811110000000006</v>
       </c>
-      <c r="S17" s="151">
+      <c r="S17" s="146">
         <f t="shared" si="16"/>
-        <v>104.47600639594387</v>
-      </c>
-      <c r="T17" s="170">
+        <v>103.98772071014974</v>
+      </c>
+      <c r="T17" s="165">
         <f>N17*10^3/S17</f>
-        <v>524.16819793492891</v>
-      </c>
-      <c r="U17" s="153"/>
-      <c r="V17" s="154">
+        <v>526.6294868857035</v>
+      </c>
+      <c r="U17" s="148"/>
+      <c r="V17" s="149">
         <f>($T$18-T17)^2</f>
-        <v>129.84513219581763</v>
-      </c>
-      <c r="X17" s="193"/>
-      <c r="Y17" s="177">
+        <v>131.06739908199424</v>
+      </c>
+      <c r="X17" s="188"/>
+      <c r="Y17" s="172">
         <v>620</v>
       </c>
-      <c r="Z17" s="196"/>
-      <c r="AA17" s="165">
+      <c r="Z17" s="191"/>
+      <c r="AA17" s="160">
         <f t="shared" si="17"/>
         <v>1476.2199999999998</v>
       </c>
-      <c r="AB17" s="166">
+      <c r="AB17" s="161">
         <v>133.5</v>
       </c>
-      <c r="AC17" s="164">
+      <c r="AC17" s="159">
         <f t="shared" ref="AC17" si="21">AB17*$B$2/10</f>
         <v>150.98849999999999</v>
       </c>
-      <c r="AD17" s="166">
+      <c r="AD17" s="161">
         <v>135.30000000000001</v>
       </c>
-      <c r="AE17" s="164">
+      <c r="AE17" s="159">
         <f t="shared" ref="AE17" si="22">AD17*$B$2/10</f>
         <v>153.02430000000001</v>
       </c>
-      <c r="AF17" s="169">
+      <c r="AF17" s="164">
         <f>(($F$9/COS(RADIANS(0))*AC17)+(1/COS(RADIANS(15)*AE17)))</f>
         <v>146.74501411526421</v>
       </c>
-      <c r="AG17" s="199">
+      <c r="AG17" s="194">
         <f>AA17*10^3/AF17</f>
         <v>10059.762567745362</v>
       </c>
-      <c r="AH17" s="153"/>
-      <c r="AI17" s="156"/>
-      <c r="AK17" s="171"/>
-      <c r="AL17" s="177">
+      <c r="AH17" s="148"/>
+      <c r="AI17" s="151"/>
+      <c r="AK17" s="166"/>
+      <c r="AL17" s="172">
         <v>570</v>
       </c>
-      <c r="AM17" s="178" t="s">
+      <c r="AM17" s="173" t="s">
         <v>74</v>
       </c>
-      <c r="AN17" s="165" t="e">
+      <c r="AN17" s="160" t="e">
         <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AO17" s="166">
+      <c r="AO17" s="161">
         <v>139.5</v>
       </c>
-      <c r="AP17" s="164">
+      <c r="AP17" s="159">
         <f t="shared" ref="AP17" si="23">AO17*$B$2/10</f>
         <v>157.77450000000002</v>
       </c>
-      <c r="AQ17" s="166">
+      <c r="AQ17" s="161">
         <v>141.5</v>
       </c>
-      <c r="AR17" s="164">
+      <c r="AR17" s="159">
         <f t="shared" ref="AR17" si="24">AQ17*$B$2/10</f>
         <v>160.03649999999999</v>
       </c>
-      <c r="AS17" s="169">
+      <c r="AS17" s="164">
         <f>(($F$9/COS(RADIANS(0))*AP17)+(1/COS(RADIANS(15)*AR17)))</f>
         <v>152.7750043830697</v>
       </c>
-      <c r="AT17" s="203" t="e">
+      <c r="AT17" s="198" t="e">
         <f>AN17*10^3/AS17</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AU17" s="153"/>
-      <c r="AV17" s="156"/>
+      <c r="AU17" s="148"/>
+      <c r="AV17" s="151"/>
     </row>
     <row r="18" spans="11:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K18" s="172"/>
-      <c r="L18" s="153"/>
-      <c r="M18" s="153"/>
-      <c r="N18" s="153"/>
-      <c r="O18" s="153"/>
-      <c r="P18" s="153"/>
-      <c r="Q18" s="153"/>
-      <c r="R18" s="153"/>
-      <c r="S18" s="153"/>
-      <c r="T18" s="179">
+      <c r="K18" s="167"/>
+      <c r="L18" s="148"/>
+      <c r="M18" s="148"/>
+      <c r="N18" s="148"/>
+      <c r="O18" s="148"/>
+      <c r="P18" s="148"/>
+      <c r="Q18" s="148"/>
+      <c r="R18" s="148"/>
+      <c r="S18" s="148"/>
+      <c r="T18" s="174">
         <f>SUM(T16:T17)/2</f>
-        <v>512.77323711025656</v>
-      </c>
-      <c r="U18" s="174" t="s">
+        <v>515.18101977949254</v>
+      </c>
+      <c r="U18" s="169" t="s">
         <v>48</v>
       </c>
-      <c r="V18" s="180">
+      <c r="V18" s="175">
         <f>SQRT(SUM(V16:V17))</f>
-        <v>16.114908140961788</v>
-      </c>
-      <c r="X18" s="176"/>
+        <v>16.190577449985792</v>
+      </c>
+      <c r="X18" s="171"/>
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
       <c r="AA18" s="3"/>
@@ -5229,9 +5253,9 @@
       <c r="AE18" s="3"/>
       <c r="AF18" s="3"/>
       <c r="AG18" s="3"/>
-      <c r="AH18" s="153"/>
-      <c r="AI18" s="156"/>
-      <c r="AK18" s="176"/>
+      <c r="AH18" s="148"/>
+      <c r="AI18" s="151"/>
+      <c r="AK18" s="171"/>
       <c r="AL18" s="3"/>
       <c r="AM18" s="3"/>
       <c r="AN18" s="3"/>
@@ -5240,24 +5264,24 @@
       <c r="AQ18" s="3"/>
       <c r="AR18" s="3"/>
       <c r="AS18" s="3"/>
-      <c r="AT18" s="200"/>
-      <c r="AU18" s="153"/>
-      <c r="AV18" s="156"/>
+      <c r="AT18" s="195"/>
+      <c r="AU18" s="148"/>
+      <c r="AV18" s="151"/>
     </row>
     <row r="19" spans="11:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K19" s="172"/>
-      <c r="L19" s="153"/>
-      <c r="M19" s="153"/>
-      <c r="N19" s="153"/>
-      <c r="O19" s="153"/>
-      <c r="P19" s="153"/>
-      <c r="Q19" s="153"/>
-      <c r="R19" s="153"/>
-      <c r="S19" s="153"/>
-      <c r="T19" s="153"/>
-      <c r="U19" s="153"/>
-      <c r="V19" s="156"/>
-      <c r="X19" s="176"/>
+      <c r="K19" s="167"/>
+      <c r="L19" s="148"/>
+      <c r="M19" s="148"/>
+      <c r="N19" s="148"/>
+      <c r="O19" s="148"/>
+      <c r="P19" s="148"/>
+      <c r="Q19" s="148"/>
+      <c r="R19" s="148"/>
+      <c r="S19" s="148"/>
+      <c r="T19" s="148"/>
+      <c r="U19" s="148"/>
+      <c r="V19" s="151"/>
+      <c r="X19" s="171"/>
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
       <c r="AA19" s="3"/>
@@ -5267,9 +5291,9 @@
       <c r="AE19" s="3"/>
       <c r="AF19" s="3"/>
       <c r="AG19" s="3"/>
-      <c r="AH19" s="153"/>
-      <c r="AI19" s="156"/>
-      <c r="AK19" s="176"/>
+      <c r="AH19" s="148"/>
+      <c r="AI19" s="151"/>
+      <c r="AK19" s="171"/>
       <c r="AL19" s="3"/>
       <c r="AM19" s="3"/>
       <c r="AN19" s="3"/>
@@ -5278,1682 +5302,1682 @@
       <c r="AQ19" s="3"/>
       <c r="AR19" s="3"/>
       <c r="AS19" s="3"/>
-      <c r="AT19" s="200"/>
-      <c r="AU19" s="153"/>
-      <c r="AV19" s="156"/>
+      <c r="AT19" s="195"/>
+      <c r="AU19" s="148"/>
+      <c r="AV19" s="151"/>
     </row>
     <row r="20" spans="11:48" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K20" s="132" t="s">
+      <c r="K20" s="127" t="s">
         <v>75</v>
       </c>
-      <c r="L20" s="133" t="s">
+      <c r="L20" s="128" t="s">
         <v>54</v>
       </c>
-      <c r="M20" s="134" t="s">
+      <c r="M20" s="129" t="s">
         <v>55</v>
       </c>
-      <c r="N20" s="135" t="s">
+      <c r="N20" s="130" t="s">
         <v>56</v>
       </c>
-      <c r="O20" s="134" t="s">
+      <c r="O20" s="129" t="s">
         <v>57</v>
       </c>
-      <c r="P20" s="135" t="s">
+      <c r="P20" s="130" t="s">
         <v>58</v>
       </c>
-      <c r="Q20" s="134" t="s">
+      <c r="Q20" s="129" t="s">
         <v>59</v>
       </c>
-      <c r="R20" s="135" t="s">
+      <c r="R20" s="130" t="s">
         <v>60</v>
       </c>
-      <c r="S20" s="136" t="s">
+      <c r="S20" s="131" t="s">
         <v>61</v>
       </c>
-      <c r="T20" s="137" t="s">
+      <c r="T20" s="132" t="s">
         <v>62</v>
       </c>
-      <c r="U20" s="153"/>
-      <c r="V20" s="156"/>
-      <c r="X20" s="186"/>
-      <c r="Y20" s="187" t="s">
+      <c r="U20" s="148"/>
+      <c r="V20" s="151"/>
+      <c r="X20" s="181"/>
+      <c r="Y20" s="182" t="s">
         <v>65</v>
       </c>
-      <c r="Z20" s="188" t="s">
+      <c r="Z20" s="183" t="s">
         <v>66</v>
       </c>
-      <c r="AA20" s="188" t="s">
+      <c r="AA20" s="183" t="s">
         <v>56</v>
       </c>
-      <c r="AB20" s="188" t="s">
+      <c r="AB20" s="183" t="s">
         <v>57</v>
       </c>
-      <c r="AC20" s="188" t="s">
+      <c r="AC20" s="183" t="s">
         <v>58</v>
       </c>
-      <c r="AD20" s="188" t="s">
+      <c r="AD20" s="183" t="s">
         <v>59</v>
       </c>
-      <c r="AE20" s="188" t="s">
+      <c r="AE20" s="183" t="s">
         <v>60</v>
       </c>
-      <c r="AF20" s="189" t="s">
+      <c r="AF20" s="184" t="s">
         <v>61</v>
       </c>
-      <c r="AG20" s="190" t="s">
+      <c r="AG20" s="185" t="s">
         <v>62</v>
       </c>
-      <c r="AH20" s="153"/>
-      <c r="AI20" s="156"/>
-      <c r="AK20" s="140"/>
-      <c r="AL20" s="141" t="s">
+      <c r="AH20" s="148"/>
+      <c r="AI20" s="151"/>
+      <c r="AK20" s="135"/>
+      <c r="AL20" s="136" t="s">
         <v>63</v>
       </c>
-      <c r="AM20" s="142" t="s">
+      <c r="AM20" s="137" t="s">
         <v>64</v>
       </c>
-      <c r="AN20" s="142" t="s">
+      <c r="AN20" s="137" t="s">
         <v>56</v>
       </c>
-      <c r="AO20" s="142" t="s">
+      <c r="AO20" s="137" t="s">
         <v>57</v>
       </c>
-      <c r="AP20" s="142" t="s">
+      <c r="AP20" s="137" t="s">
         <v>58</v>
       </c>
-      <c r="AQ20" s="142" t="s">
+      <c r="AQ20" s="137" t="s">
         <v>59</v>
       </c>
-      <c r="AR20" s="142" t="s">
+      <c r="AR20" s="137" t="s">
         <v>60</v>
       </c>
-      <c r="AS20" s="143" t="s">
+      <c r="AS20" s="138" t="s">
         <v>61</v>
       </c>
-      <c r="AT20" s="201" t="s">
+      <c r="AT20" s="196" t="s">
         <v>62</v>
       </c>
-      <c r="AU20" s="153"/>
-      <c r="AV20" s="156"/>
+      <c r="AU20" s="148"/>
+      <c r="AV20" s="151"/>
     </row>
     <row r="21" spans="11:48" x14ac:dyDescent="0.35">
-      <c r="K21" s="145" t="s">
+      <c r="K21" s="140" t="s">
         <v>76</v>
       </c>
-      <c r="L21" s="181">
+      <c r="L21" s="176">
         <v>809</v>
       </c>
-      <c r="M21" s="147">
+      <c r="M21" s="142">
         <v>768</v>
       </c>
-      <c r="N21" s="148">
+      <c r="N21" s="143">
         <f>(L21-M21)*2.381</f>
         <v>97.620999999999995</v>
       </c>
-      <c r="O21" s="147">
+      <c r="O21" s="142">
+        <v>45.37</v>
+      </c>
+      <c r="P21" s="142">
+        <f>O21*$B$2/10</f>
+        <v>51.313469999999995</v>
+      </c>
+      <c r="Q21" s="142">
         <v>45.81</v>
       </c>
-      <c r="P21" s="147">
-        <f>O21*$B$2/10</f>
-        <v>51.811110000000006</v>
-      </c>
-      <c r="Q21" s="147">
-        <v>45.81</v>
-      </c>
-      <c r="R21" s="147">
+      <c r="R21" s="142">
         <f>Q21*$B$2/10</f>
         <v>51.811110000000006</v>
       </c>
-      <c r="S21" s="151">
+      <c r="S21" s="146">
         <f t="shared" ref="S21:S22" si="25">(($F$9/COS(RADIANS(0))*P21)+(1/COS(RADIANS(15))*R21))</f>
-        <v>104.47600639594387</v>
-      </c>
-      <c r="T21" s="152">
+        <v>103.98772071014974</v>
+      </c>
+      <c r="T21" s="147">
         <f>N21*10^3/S21</f>
-        <v>934.38678762313407</v>
-      </c>
-      <c r="U21" s="153"/>
-      <c r="V21" s="154">
+        <v>938.77430270929744</v>
+      </c>
+      <c r="U21" s="148"/>
+      <c r="V21" s="149">
         <f>($T$23-T21)^2</f>
-        <v>1168.6061897623586</v>
-      </c>
-      <c r="X21" s="191"/>
-      <c r="Y21" s="182">
+        <v>1179.6065917379483</v>
+      </c>
+      <c r="X21" s="186"/>
+      <c r="Y21" s="177">
         <v>605</v>
       </c>
-      <c r="Z21" s="147"/>
-      <c r="AA21" s="148">
+      <c r="Z21" s="142"/>
+      <c r="AA21" s="143">
         <f t="shared" ref="AA21:AA22" si="26">(Y21-Z21)*2.381</f>
         <v>1440.5049999999999</v>
       </c>
-      <c r="AB21" s="147">
+      <c r="AB21" s="142">
         <v>133.5</v>
       </c>
-      <c r="AC21" s="147">
+      <c r="AC21" s="142">
         <f>AB21*$B$2/10</f>
         <v>150.98849999999999</v>
       </c>
-      <c r="AD21" s="147">
+      <c r="AD21" s="142">
         <v>135.30000000000001</v>
       </c>
-      <c r="AE21" s="147">
+      <c r="AE21" s="142">
         <f>AD21*$B$2/10</f>
         <v>153.02430000000001</v>
       </c>
-      <c r="AF21" s="151">
+      <c r="AF21" s="146">
         <f>(($F$9/COS(RADIANS(0))*AC21)+(1/COS(RADIANS(15)*AE21)))</f>
         <v>146.74501411526421</v>
       </c>
-      <c r="AG21" s="197">
+      <c r="AG21" s="192">
         <f>AA21*10^3/AF21</f>
         <v>9816.3812152999108</v>
       </c>
-      <c r="AH21" s="153"/>
-      <c r="AI21" s="156"/>
-      <c r="AK21" s="155"/>
-      <c r="AL21" s="194">
+      <c r="AH21" s="148"/>
+      <c r="AI21" s="151"/>
+      <c r="AK21" s="150"/>
+      <c r="AL21" s="189">
         <v>555</v>
       </c>
-      <c r="AM21" s="195" t="s">
+      <c r="AM21" s="190" t="s">
         <v>77</v>
       </c>
-      <c r="AN21" s="148" t="e">
+      <c r="AN21" s="143" t="e">
         <f t="shared" ref="AN21:AN22" si="27">(AL21-AM21)*2.381</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AO21" s="147">
+      <c r="AO21" s="142">
         <v>139.5</v>
       </c>
-      <c r="AP21" s="147">
+      <c r="AP21" s="142">
         <f>AO21*$B$2/10</f>
         <v>157.77450000000002</v>
       </c>
-      <c r="AQ21" s="147">
+      <c r="AQ21" s="142">
         <v>141.5</v>
       </c>
-      <c r="AR21" s="147">
+      <c r="AR21" s="142">
         <f>AQ21*$B$2/10</f>
         <v>160.03649999999999</v>
       </c>
-      <c r="AS21" s="151">
+      <c r="AS21" s="146">
         <f>(($F$9/COS(RADIANS(0))*AP21)+(1/COS(RADIANS(15)*AR21)))</f>
         <v>152.7750043830697</v>
       </c>
-      <c r="AT21" s="197" t="e">
+      <c r="AT21" s="192" t="e">
         <f>AN21*10^3/AS21</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AU21" s="153"/>
-      <c r="AV21" s="156"/>
+      <c r="AU21" s="148"/>
+      <c r="AV21" s="151"/>
     </row>
     <row r="22" spans="11:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K22" s="162" t="s">
+      <c r="K22" s="157" t="s">
         <v>78</v>
       </c>
-      <c r="L22" s="163">
+      <c r="L22" s="158">
         <v>811</v>
       </c>
-      <c r="M22" s="164">
+      <c r="M22" s="159">
         <v>767</v>
       </c>
-      <c r="N22" s="165">
+      <c r="N22" s="160">
         <f>(L22-M22)*2.381</f>
         <v>104.764</v>
       </c>
-      <c r="O22" s="166">
+      <c r="O22" s="161">
+        <v>45.37</v>
+      </c>
+      <c r="P22" s="159">
+        <f>O22*$B$2/10</f>
+        <v>51.313469999999995</v>
+      </c>
+      <c r="Q22" s="161">
         <v>45.81</v>
       </c>
-      <c r="P22" s="164">
-        <f>O22*$B$2/10</f>
-        <v>51.811110000000006</v>
-      </c>
-      <c r="Q22" s="166">
-        <v>45.81</v>
-      </c>
-      <c r="R22" s="164">
+      <c r="R22" s="159">
         <f>Q22*$B$2/10</f>
         <v>51.811110000000006</v>
       </c>
-      <c r="S22" s="151">
+      <c r="S22" s="146">
         <f t="shared" si="25"/>
-        <v>104.47600639594387</v>
-      </c>
-      <c r="T22" s="170">
+        <v>103.98772071014974</v>
+      </c>
+      <c r="T22" s="165">
         <f>N22*10^3/S22</f>
-        <v>1002.7565525711683</v>
-      </c>
-      <c r="U22" s="153"/>
-      <c r="V22" s="154">
+        <v>1007.4651053465632</v>
+      </c>
+      <c r="U22" s="148"/>
+      <c r="V22" s="149">
         <f>($T$23-T22)^2</f>
-        <v>1168.6061897623665</v>
-      </c>
-      <c r="X22" s="193"/>
-      <c r="Y22" s="163">
+        <v>1179.6065917379483</v>
+      </c>
+      <c r="X22" s="188"/>
+      <c r="Y22" s="158">
         <v>610</v>
       </c>
-      <c r="Z22" s="164">
+      <c r="Z22" s="159">
         <v>590</v>
       </c>
-      <c r="AA22" s="165">
+      <c r="AA22" s="160">
         <f t="shared" si="26"/>
         <v>47.62</v>
       </c>
-      <c r="AB22" s="166">
+      <c r="AB22" s="161">
         <v>133.5</v>
       </c>
-      <c r="AC22" s="164">
+      <c r="AC22" s="159">
         <f t="shared" ref="AC22" si="28">AB22*$B$2/10</f>
         <v>150.98849999999999</v>
       </c>
-      <c r="AD22" s="166">
+      <c r="AD22" s="161">
         <v>135.30000000000001</v>
       </c>
-      <c r="AE22" s="164">
+      <c r="AE22" s="159">
         <f t="shared" ref="AE22" si="29">AD22*$B$2/10</f>
         <v>153.02430000000001</v>
       </c>
-      <c r="AF22" s="169">
+      <c r="AF22" s="164">
         <f>(($F$9/COS(RADIANS(0))*AC22)+(1/COS(RADIANS(15)*AE22)))</f>
         <v>146.74501411526421</v>
       </c>
-      <c r="AG22" s="199">
+      <c r="AG22" s="194">
         <f>AA22*10^3/AF22</f>
         <v>324.5084699272698</v>
       </c>
-      <c r="AH22" s="153"/>
-      <c r="AI22" s="156"/>
-      <c r="AK22" s="171"/>
-      <c r="AL22" s="177">
+      <c r="AH22" s="148"/>
+      <c r="AI22" s="151"/>
+      <c r="AK22" s="166"/>
+      <c r="AL22" s="172">
         <v>555</v>
       </c>
-      <c r="AM22" s="178">
+      <c r="AM22" s="173">
         <v>536</v>
       </c>
-      <c r="AN22" s="165">
+      <c r="AN22" s="160">
         <f t="shared" si="27"/>
         <v>45.238999999999997</v>
       </c>
-      <c r="AO22" s="166">
+      <c r="AO22" s="161">
         <v>139.5</v>
       </c>
-      <c r="AP22" s="164">
+      <c r="AP22" s="159">
         <f t="shared" ref="AP22" si="30">AO22*$B$2/10</f>
         <v>157.77450000000002</v>
       </c>
-      <c r="AQ22" s="166">
+      <c r="AQ22" s="161">
         <v>141.5</v>
       </c>
-      <c r="AR22" s="164">
+      <c r="AR22" s="159">
         <f t="shared" ref="AR22" si="31">AQ22*$B$2/10</f>
         <v>160.03649999999999</v>
       </c>
-      <c r="AS22" s="169">
+      <c r="AS22" s="164">
         <f>(($F$9/COS(RADIANS(0))*AP22)+(1/COS(RADIANS(15)*AR22)))</f>
         <v>152.7750043830697</v>
       </c>
-      <c r="AT22" s="199">
+      <c r="AT22" s="194">
         <f>AN22*10^3/AS22</f>
         <v>296.11519359912597</v>
       </c>
-      <c r="AU22" s="153"/>
-      <c r="AV22" s="156"/>
+      <c r="AU22" s="148"/>
+      <c r="AV22" s="151"/>
     </row>
     <row r="23" spans="11:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K23" s="183"/>
-      <c r="L23" s="184"/>
-      <c r="M23" s="184"/>
-      <c r="N23" s="184"/>
-      <c r="O23" s="184"/>
-      <c r="P23" s="184"/>
-      <c r="Q23" s="184"/>
-      <c r="R23" s="184"/>
-      <c r="S23" s="184"/>
-      <c r="T23" s="179">
+      <c r="K23" s="178"/>
+      <c r="L23" s="179"/>
+      <c r="M23" s="179"/>
+      <c r="N23" s="179"/>
+      <c r="O23" s="179"/>
+      <c r="P23" s="179"/>
+      <c r="Q23" s="179"/>
+      <c r="R23" s="179"/>
+      <c r="S23" s="179"/>
+      <c r="T23" s="174">
         <f>SUM(T21:T22)/2</f>
-        <v>968.57167009715113</v>
-      </c>
-      <c r="U23" s="174" t="s">
+        <v>973.11970402793031</v>
+      </c>
+      <c r="U23" s="169" t="s">
         <v>48</v>
       </c>
-      <c r="V23" s="180">
+      <c r="V23" s="175">
         <f>SQRT(SUM(V21:V22))</f>
-        <v>48.344724422885328</v>
-      </c>
-      <c r="X23" s="183"/>
-      <c r="Y23" s="184"/>
-      <c r="Z23" s="184"/>
-      <c r="AA23" s="184"/>
-      <c r="AB23" s="184"/>
-      <c r="AC23" s="184"/>
-      <c r="AD23" s="184"/>
-      <c r="AE23" s="184"/>
-      <c r="AF23" s="184"/>
-      <c r="AG23" s="184"/>
-      <c r="AH23" s="184"/>
-      <c r="AI23" s="185"/>
-      <c r="AK23" s="183"/>
-      <c r="AL23" s="184"/>
-      <c r="AM23" s="184"/>
-      <c r="AN23" s="184"/>
-      <c r="AO23" s="184"/>
-      <c r="AP23" s="184"/>
-      <c r="AQ23" s="184"/>
-      <c r="AR23" s="184"/>
-      <c r="AS23" s="184"/>
-      <c r="AT23" s="184"/>
-      <c r="AU23" s="184"/>
-      <c r="AV23" s="185"/>
+        <v>48.571732349957387</v>
+      </c>
+      <c r="X23" s="178"/>
+      <c r="Y23" s="179"/>
+      <c r="Z23" s="179"/>
+      <c r="AA23" s="179"/>
+      <c r="AB23" s="179"/>
+      <c r="AC23" s="179"/>
+      <c r="AD23" s="179"/>
+      <c r="AE23" s="179"/>
+      <c r="AF23" s="179"/>
+      <c r="AG23" s="179"/>
+      <c r="AH23" s="179"/>
+      <c r="AI23" s="180"/>
+      <c r="AK23" s="178"/>
+      <c r="AL23" s="179"/>
+      <c r="AM23" s="179"/>
+      <c r="AN23" s="179"/>
+      <c r="AO23" s="179"/>
+      <c r="AP23" s="179"/>
+      <c r="AQ23" s="179"/>
+      <c r="AR23" s="179"/>
+      <c r="AS23" s="179"/>
+      <c r="AT23" s="179"/>
+      <c r="AU23" s="179"/>
+      <c r="AV23" s="180"/>
     </row>
     <row r="24" spans="11:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K24" s="172"/>
-      <c r="L24" s="153"/>
-      <c r="M24" s="153"/>
-      <c r="N24" s="153"/>
-      <c r="O24" s="153"/>
-      <c r="P24" s="153"/>
-      <c r="Q24" s="153"/>
-      <c r="R24" s="153"/>
-      <c r="S24" s="153"/>
-      <c r="T24" s="153"/>
-      <c r="U24" s="153"/>
-      <c r="V24" s="156"/>
-      <c r="X24" s="172"/>
-      <c r="Y24" s="153"/>
-      <c r="Z24" s="153"/>
-      <c r="AA24" s="153"/>
-      <c r="AB24" s="153"/>
-      <c r="AC24" s="153"/>
-      <c r="AD24" s="153"/>
-      <c r="AE24" s="153"/>
-      <c r="AF24" s="153"/>
-      <c r="AG24" s="153"/>
-      <c r="AH24" s="153"/>
-      <c r="AI24" s="156"/>
-      <c r="AK24" s="172"/>
-      <c r="AL24" s="153"/>
-      <c r="AM24" s="153"/>
-      <c r="AN24" s="153"/>
-      <c r="AO24" s="153"/>
-      <c r="AP24" s="153"/>
-      <c r="AQ24" s="153"/>
-      <c r="AR24" s="153"/>
-      <c r="AS24" s="153"/>
-      <c r="AT24" s="153"/>
-      <c r="AU24" s="153"/>
-      <c r="AV24" s="156"/>
+      <c r="K24" s="167"/>
+      <c r="L24" s="148"/>
+      <c r="M24" s="148"/>
+      <c r="N24" s="148"/>
+      <c r="O24" s="148"/>
+      <c r="P24" s="148"/>
+      <c r="Q24" s="148"/>
+      <c r="R24" s="148"/>
+      <c r="S24" s="148"/>
+      <c r="T24" s="148"/>
+      <c r="U24" s="148"/>
+      <c r="V24" s="151"/>
+      <c r="X24" s="167"/>
+      <c r="Y24" s="148"/>
+      <c r="Z24" s="148"/>
+      <c r="AA24" s="148"/>
+      <c r="AB24" s="148"/>
+      <c r="AC24" s="148"/>
+      <c r="AD24" s="148"/>
+      <c r="AE24" s="148"/>
+      <c r="AF24" s="148"/>
+      <c r="AG24" s="148"/>
+      <c r="AH24" s="148"/>
+      <c r="AI24" s="151"/>
+      <c r="AK24" s="167"/>
+      <c r="AL24" s="148"/>
+      <c r="AM24" s="148"/>
+      <c r="AN24" s="148"/>
+      <c r="AO24" s="148"/>
+      <c r="AP24" s="148"/>
+      <c r="AQ24" s="148"/>
+      <c r="AR24" s="148"/>
+      <c r="AS24" s="148"/>
+      <c r="AT24" s="148"/>
+      <c r="AU24" s="148"/>
+      <c r="AV24" s="151"/>
     </row>
     <row r="25" spans="11:48" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K25" s="132" t="s">
+      <c r="K25" s="127" t="s">
         <v>79</v>
       </c>
-      <c r="L25" s="133" t="s">
+      <c r="L25" s="128" t="s">
         <v>54</v>
       </c>
-      <c r="M25" s="134" t="s">
+      <c r="M25" s="129" t="s">
         <v>55</v>
       </c>
-      <c r="N25" s="135" t="s">
+      <c r="N25" s="130" t="s">
         <v>56</v>
       </c>
-      <c r="O25" s="134" t="s">
+      <c r="O25" s="129" t="s">
         <v>57</v>
       </c>
-      <c r="P25" s="135" t="s">
+      <c r="P25" s="130" t="s">
         <v>58</v>
       </c>
-      <c r="Q25" s="134" t="s">
+      <c r="Q25" s="129" t="s">
         <v>59</v>
       </c>
-      <c r="R25" s="135" t="s">
+      <c r="R25" s="130" t="s">
         <v>60</v>
       </c>
-      <c r="S25" s="136" t="s">
+      <c r="S25" s="131" t="s">
         <v>61</v>
       </c>
-      <c r="T25" s="137" t="s">
+      <c r="T25" s="132" t="s">
         <v>62</v>
       </c>
-      <c r="U25" s="153"/>
-      <c r="V25" s="156"/>
-      <c r="X25" s="186"/>
-      <c r="Y25" s="187" t="s">
+      <c r="U25" s="148"/>
+      <c r="V25" s="151"/>
+      <c r="X25" s="181"/>
+      <c r="Y25" s="182" t="s">
         <v>65</v>
       </c>
-      <c r="Z25" s="188" t="s">
+      <c r="Z25" s="183" t="s">
         <v>66</v>
       </c>
-      <c r="AA25" s="188" t="s">
+      <c r="AA25" s="183" t="s">
         <v>56</v>
       </c>
-      <c r="AB25" s="188" t="s">
+      <c r="AB25" s="183" t="s">
         <v>57</v>
       </c>
-      <c r="AC25" s="188" t="s">
+      <c r="AC25" s="183" t="s">
         <v>58</v>
       </c>
-      <c r="AD25" s="188" t="s">
+      <c r="AD25" s="183" t="s">
         <v>59</v>
       </c>
-      <c r="AE25" s="188" t="s">
+      <c r="AE25" s="183" t="s">
         <v>60</v>
       </c>
-      <c r="AF25" s="189" t="s">
+      <c r="AF25" s="184" t="s">
         <v>61</v>
       </c>
-      <c r="AG25" s="190" t="s">
+      <c r="AG25" s="185" t="s">
         <v>62</v>
       </c>
-      <c r="AH25" s="153"/>
-      <c r="AI25" s="156"/>
-      <c r="AK25" s="140"/>
-      <c r="AL25" s="141" t="s">
+      <c r="AH25" s="148"/>
+      <c r="AI25" s="151"/>
+      <c r="AK25" s="135"/>
+      <c r="AL25" s="136" t="s">
         <v>63</v>
       </c>
-      <c r="AM25" s="142" t="s">
+      <c r="AM25" s="137" t="s">
         <v>64</v>
       </c>
-      <c r="AN25" s="142" t="s">
+      <c r="AN25" s="137" t="s">
         <v>56</v>
       </c>
-      <c r="AO25" s="142" t="s">
+      <c r="AO25" s="137" t="s">
         <v>57</v>
       </c>
-      <c r="AP25" s="142" t="s">
+      <c r="AP25" s="137" t="s">
         <v>58</v>
       </c>
-      <c r="AQ25" s="142" t="s">
+      <c r="AQ25" s="137" t="s">
         <v>59</v>
       </c>
-      <c r="AR25" s="142" t="s">
+      <c r="AR25" s="137" t="s">
         <v>60</v>
       </c>
-      <c r="AS25" s="143" t="s">
+      <c r="AS25" s="138" t="s">
         <v>61</v>
       </c>
-      <c r="AT25" s="201" t="s">
+      <c r="AT25" s="196" t="s">
         <v>62</v>
       </c>
-      <c r="AU25" s="153"/>
-      <c r="AV25" s="156"/>
+      <c r="AU25" s="148"/>
+      <c r="AV25" s="151"/>
     </row>
     <row r="26" spans="11:48" x14ac:dyDescent="0.35">
-      <c r="K26" s="145" t="s">
+      <c r="K26" s="140" t="s">
         <v>80</v>
       </c>
-      <c r="L26" s="181">
+      <c r="L26" s="176">
         <v>810</v>
       </c>
-      <c r="M26" s="147">
+      <c r="M26" s="142">
         <v>782</v>
       </c>
-      <c r="N26" s="148">
+      <c r="N26" s="143">
         <f>(L26-M26)*2.381</f>
         <v>66.667999999999992</v>
       </c>
-      <c r="O26" s="147">
+      <c r="O26" s="142">
+        <v>45.37</v>
+      </c>
+      <c r="P26" s="142">
+        <f>O26*$B$2/10</f>
+        <v>51.313469999999995</v>
+      </c>
+      <c r="Q26" s="142">
         <v>45.81</v>
       </c>
-      <c r="P26" s="147">
-        <f>O26*$B$2/10</f>
-        <v>51.811110000000006</v>
-      </c>
-      <c r="Q26" s="147">
-        <v>45.81</v>
-      </c>
-      <c r="R26" s="147">
+      <c r="R26" s="142">
         <f>Q26*$B$2/10</f>
         <v>51.811110000000006</v>
       </c>
-      <c r="S26" s="151">
+      <c r="S26" s="146">
         <f t="shared" ref="S26:S27" si="32">(($F$9/COS(RADIANS(0))*P26)+(1/COS(RADIANS(15))*R26))</f>
-        <v>104.47600639594387</v>
-      </c>
-      <c r="T26" s="152">
+        <v>103.98772071014974</v>
+      </c>
+      <c r="T26" s="147">
         <f>N26*10^3/S26</f>
-        <v>638.11780618165244</v>
-      </c>
-      <c r="U26" s="153"/>
-      <c r="V26" s="154">
+        <v>641.11415794781283</v>
+      </c>
+      <c r="U26" s="148"/>
+      <c r="V26" s="149">
         <f>($T$28-T26)^2</f>
-        <v>519.38052878327051</v>
-      </c>
-      <c r="X26" s="191"/>
-      <c r="Y26" s="209"/>
-      <c r="Z26" s="210"/>
-      <c r="AA26" s="148">
+        <v>524.26959632797696</v>
+      </c>
+      <c r="X26" s="186"/>
+      <c r="Y26" s="204"/>
+      <c r="Z26" s="205"/>
+      <c r="AA26" s="143">
         <f>(AL26-AM26)*2.381</f>
         <v>35.714999999999996</v>
       </c>
-      <c r="AB26" s="147">
+      <c r="AB26" s="142">
         <v>133.5</v>
       </c>
-      <c r="AC26" s="147">
+      <c r="AC26" s="142">
         <f>AB26*$B$2/10</f>
         <v>150.98849999999999</v>
       </c>
-      <c r="AD26" s="147">
+      <c r="AD26" s="142">
         <v>135.30000000000001</v>
       </c>
-      <c r="AE26" s="147">
+      <c r="AE26" s="142">
         <f>AD26*$B$2/10</f>
         <v>153.02430000000001</v>
       </c>
-      <c r="AF26" s="151">
+      <c r="AF26" s="146">
         <f>(($F$9/COS(RADIANS(0))*AC26)+(1/COS(RADIANS(15)*AE26)))</f>
         <v>146.74501411526421</v>
       </c>
-      <c r="AG26" s="197">
+      <c r="AG26" s="192">
         <f>AA26*10^3/AF26</f>
         <v>243.38135244545231</v>
       </c>
-      <c r="AH26" s="153"/>
-      <c r="AI26" s="156"/>
-      <c r="AK26" s="155"/>
-      <c r="AL26" s="182">
+      <c r="AH26" s="148"/>
+      <c r="AI26" s="151"/>
+      <c r="AK26" s="150"/>
+      <c r="AL26" s="177">
         <v>569</v>
       </c>
-      <c r="AM26" s="147">
+      <c r="AM26" s="142">
         <v>554</v>
       </c>
-      <c r="AN26" s="148" t="e">
+      <c r="AN26" s="143" t="e">
         <f>(#REF!-#REF!)*2.381</f>
         <v>#REF!</v>
       </c>
-      <c r="AO26" s="147">
+      <c r="AO26" s="142">
         <v>139.5</v>
       </c>
-      <c r="AP26" s="147">
+      <c r="AP26" s="142">
         <f>AO26*$B$2/10</f>
         <v>157.77450000000002</v>
       </c>
-      <c r="AQ26" s="147">
+      <c r="AQ26" s="142">
         <v>141.5</v>
       </c>
-      <c r="AR26" s="147">
+      <c r="AR26" s="142">
         <f>AQ26*$B$2/10</f>
         <v>160.03649999999999</v>
       </c>
-      <c r="AS26" s="151">
+      <c r="AS26" s="146">
         <f>(($F$9/COS(RADIANS(0))*AP26)+(1/COS(RADIANS(15)*AR26)))</f>
         <v>152.7750043830697</v>
       </c>
-      <c r="AT26" s="197" t="e">
+      <c r="AT26" s="192" t="e">
         <f>AN26*10^3/AS26</f>
         <v>#REF!</v>
       </c>
-      <c r="AU26" s="153"/>
-      <c r="AV26" s="156"/>
+      <c r="AU26" s="148"/>
+      <c r="AV26" s="151"/>
     </row>
     <row r="27" spans="11:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K27" s="162" t="s">
+      <c r="K27" s="157" t="s">
         <v>86</v>
       </c>
-      <c r="L27" s="163">
+      <c r="L27" s="158">
         <v>810</v>
       </c>
-      <c r="M27" s="164">
+      <c r="M27" s="159">
         <v>780</v>
       </c>
-      <c r="N27" s="165">
+      <c r="N27" s="160">
         <f>(L27-M27)*2.381</f>
         <v>71.429999999999993</v>
       </c>
-      <c r="O27" s="166">
+      <c r="O27" s="161">
+        <v>45.37</v>
+      </c>
+      <c r="P27" s="159">
+        <f>O27*$B$2/10</f>
+        <v>51.313469999999995</v>
+      </c>
+      <c r="Q27" s="161">
         <v>45.81</v>
       </c>
-      <c r="P27" s="164">
-        <f>O27*$B$2/10</f>
-        <v>51.811110000000006</v>
-      </c>
-      <c r="Q27" s="166">
-        <v>45.81</v>
-      </c>
-      <c r="R27" s="164">
+      <c r="R27" s="159">
         <f>Q27*$B$2/10</f>
         <v>51.811110000000006</v>
       </c>
-      <c r="S27" s="151">
+      <c r="S27" s="146">
         <f t="shared" si="32"/>
-        <v>104.47600639594387</v>
-      </c>
-      <c r="T27" s="170">
+        <v>103.98772071014974</v>
+      </c>
+      <c r="T27" s="165">
         <f>N27*10^3/S27</f>
-        <v>683.69764948034185</v>
-      </c>
-      <c r="U27" s="153"/>
-      <c r="V27" s="154">
+        <v>686.90802637265654</v>
+      </c>
+      <c r="U27" s="148"/>
+      <c r="V27" s="149">
         <f>($T$28-T27)^2</f>
-        <v>519.38052878327051</v>
-      </c>
-      <c r="X27" s="193"/>
-      <c r="Y27" s="163"/>
-      <c r="Z27" s="164"/>
-      <c r="AA27" s="165">
+        <v>524.26959632797184</v>
+      </c>
+      <c r="X27" s="188"/>
+      <c r="Y27" s="158"/>
+      <c r="Z27" s="159"/>
+      <c r="AA27" s="160">
         <f t="shared" ref="AA27" si="33">(Y27-Z27)*2.381</f>
         <v>0</v>
       </c>
-      <c r="AB27" s="166">
+      <c r="AB27" s="161">
         <v>133.5</v>
       </c>
-      <c r="AC27" s="164">
+      <c r="AC27" s="159">
         <f t="shared" ref="AC27" si="34">AB27*$B$2/10</f>
         <v>150.98849999999999</v>
       </c>
-      <c r="AD27" s="166">
+      <c r="AD27" s="161">
         <v>135.30000000000001</v>
       </c>
-      <c r="AE27" s="164">
+      <c r="AE27" s="159">
         <f t="shared" ref="AE27" si="35">AD27*$B$2/10</f>
         <v>153.02430000000001</v>
       </c>
-      <c r="AF27" s="169">
+      <c r="AF27" s="164">
         <f>(($F$9/COS(RADIANS(0))*AC27)+(1/COS(RADIANS(15)*AE27)))</f>
         <v>146.74501411526421</v>
       </c>
-      <c r="AG27" s="199">
+      <c r="AG27" s="194">
         <f>AA27*10^3/AF27</f>
         <v>0</v>
       </c>
-      <c r="AH27" s="153"/>
-      <c r="AI27" s="156"/>
-      <c r="AK27" s="171"/>
-      <c r="AL27" s="177"/>
-      <c r="AM27" s="178"/>
-      <c r="AN27" s="165">
+      <c r="AH27" s="148"/>
+      <c r="AI27" s="151"/>
+      <c r="AK27" s="166"/>
+      <c r="AL27" s="172"/>
+      <c r="AM27" s="173"/>
+      <c r="AN27" s="160">
         <f t="shared" ref="AN27" si="36">(AL27-AM27)*2.381</f>
         <v>0</v>
       </c>
-      <c r="AO27" s="166">
+      <c r="AO27" s="161">
         <v>139.5</v>
       </c>
-      <c r="AP27" s="164">
+      <c r="AP27" s="159">
         <f t="shared" ref="AP27" si="37">AO27*$B$2/10</f>
         <v>157.77450000000002</v>
       </c>
-      <c r="AQ27" s="166">
+      <c r="AQ27" s="161">
         <v>141.5</v>
       </c>
-      <c r="AR27" s="164">
+      <c r="AR27" s="159">
         <f t="shared" ref="AR27" si="38">AQ27*$B$2/10</f>
         <v>160.03649999999999</v>
       </c>
-      <c r="AS27" s="169">
+      <c r="AS27" s="164">
         <f>(($F$9/COS(RADIANS(0))*AP27)+(1/COS(RADIANS(15)*AR27)))</f>
         <v>152.7750043830697</v>
       </c>
-      <c r="AT27" s="199">
+      <c r="AT27" s="194">
         <f>AN27*10^3/AS27</f>
         <v>0</v>
       </c>
-      <c r="AU27" s="153"/>
-      <c r="AV27" s="156"/>
+      <c r="AU27" s="148"/>
+      <c r="AV27" s="151"/>
     </row>
     <row r="28" spans="11:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K28" s="183"/>
-      <c r="L28" s="184"/>
-      <c r="M28" s="184"/>
-      <c r="N28" s="184"/>
-      <c r="O28" s="184"/>
-      <c r="P28" s="184"/>
-      <c r="Q28" s="184"/>
-      <c r="R28" s="184"/>
-      <c r="S28" s="184"/>
-      <c r="T28" s="179">
+      <c r="K28" s="178"/>
+      <c r="L28" s="179"/>
+      <c r="M28" s="179"/>
+      <c r="N28" s="179"/>
+      <c r="O28" s="179"/>
+      <c r="P28" s="179"/>
+      <c r="Q28" s="179"/>
+      <c r="R28" s="179"/>
+      <c r="S28" s="179"/>
+      <c r="T28" s="174">
         <f>SUM(T26:T27)/2</f>
-        <v>660.90772783099715</v>
-      </c>
-      <c r="U28" s="174" t="s">
+        <v>664.01109216023474</v>
+      </c>
+      <c r="U28" s="169" t="s">
         <v>48</v>
       </c>
-      <c r="V28" s="180">
+      <c r="V28" s="175">
         <f>SQRT(SUM(V26:V27))</f>
-        <v>32.229816281923497</v>
-      </c>
-      <c r="X28" s="183"/>
-      <c r="Y28" s="184"/>
-      <c r="Z28" s="184"/>
-      <c r="AA28" s="184"/>
-      <c r="AB28" s="184"/>
-      <c r="AC28" s="184"/>
-      <c r="AD28" s="184"/>
-      <c r="AE28" s="184"/>
-      <c r="AF28" s="184"/>
-      <c r="AG28" s="184"/>
-      <c r="AH28" s="184"/>
-      <c r="AI28" s="185"/>
-      <c r="AK28" s="183"/>
-      <c r="AL28" s="184"/>
-      <c r="AM28" s="184"/>
-      <c r="AN28" s="184"/>
-      <c r="AO28" s="184"/>
-      <c r="AP28" s="184"/>
-      <c r="AQ28" s="184"/>
-      <c r="AR28" s="184"/>
-      <c r="AS28" s="184"/>
-      <c r="AT28" s="184"/>
-      <c r="AU28" s="184"/>
-      <c r="AV28" s="185"/>
+        <v>32.381154899971506</v>
+      </c>
+      <c r="X28" s="178"/>
+      <c r="Y28" s="179"/>
+      <c r="Z28" s="179"/>
+      <c r="AA28" s="179"/>
+      <c r="AB28" s="179"/>
+      <c r="AC28" s="179"/>
+      <c r="AD28" s="179"/>
+      <c r="AE28" s="179"/>
+      <c r="AF28" s="179"/>
+      <c r="AG28" s="179"/>
+      <c r="AH28" s="179"/>
+      <c r="AI28" s="180"/>
+      <c r="AK28" s="178"/>
+      <c r="AL28" s="179"/>
+      <c r="AM28" s="179"/>
+      <c r="AN28" s="179"/>
+      <c r="AO28" s="179"/>
+      <c r="AP28" s="179"/>
+      <c r="AQ28" s="179"/>
+      <c r="AR28" s="179"/>
+      <c r="AS28" s="179"/>
+      <c r="AT28" s="179"/>
+      <c r="AU28" s="179"/>
+      <c r="AV28" s="180"/>
     </row>
     <row r="30" spans="11:48" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="31" spans="11:48" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K31" s="132" t="s">
+      <c r="K31" s="127" t="s">
         <v>53</v>
       </c>
-      <c r="L31" s="133" t="s">
+      <c r="L31" s="128" t="s">
         <v>54</v>
       </c>
-      <c r="M31" s="134" t="s">
+      <c r="M31" s="129" t="s">
         <v>55</v>
       </c>
-      <c r="N31" s="135" t="s">
+      <c r="N31" s="130" t="s">
         <v>56</v>
       </c>
-      <c r="O31" s="134" t="s">
+      <c r="O31" s="129" t="s">
         <v>57</v>
       </c>
-      <c r="P31" s="135" t="s">
+      <c r="P31" s="130" t="s">
         <v>58</v>
       </c>
-      <c r="Q31" s="134" t="s">
+      <c r="Q31" s="129" t="s">
         <v>59</v>
       </c>
-      <c r="R31" s="135" t="s">
+      <c r="R31" s="130" t="s">
         <v>60</v>
       </c>
-      <c r="S31" s="136" t="s">
+      <c r="S31" s="131" t="s">
         <v>61</v>
       </c>
-      <c r="T31" s="137" t="s">
+      <c r="T31" s="132" t="s">
         <v>62</v>
       </c>
-      <c r="U31" s="138"/>
-      <c r="V31" s="139"/>
+      <c r="U31" s="133"/>
+      <c r="V31" s="134"/>
     </row>
     <row r="32" spans="11:48" x14ac:dyDescent="0.35">
-      <c r="K32" s="145" t="s">
+      <c r="K32" s="140" t="s">
         <v>82</v>
       </c>
-      <c r="L32" s="181">
+      <c r="L32" s="176">
         <v>808</v>
       </c>
-      <c r="M32" s="147">
+      <c r="M32" s="142">
         <v>728</v>
       </c>
-      <c r="N32" s="148">
+      <c r="N32" s="143">
         <f>(L32-M32)*2.381</f>
         <v>190.48</v>
       </c>
-      <c r="O32" s="147">
+      <c r="O32" s="142">
+        <v>45.37</v>
+      </c>
+      <c r="P32" s="142">
+        <f>O32*$B$2/10</f>
+        <v>51.313469999999995</v>
+      </c>
+      <c r="Q32" s="142">
         <v>45.81</v>
       </c>
-      <c r="P32" s="147">
-        <f>O32*$B$2/10</f>
-        <v>51.811110000000006</v>
-      </c>
-      <c r="Q32" s="147">
-        <v>45.81</v>
-      </c>
-      <c r="R32" s="147">
+      <c r="R32" s="142">
         <f>Q32*$B$2/10</f>
         <v>51.811110000000006</v>
       </c>
-      <c r="S32" s="151">
+      <c r="S32" s="146">
         <f t="shared" ref="S32:S33" si="39">(($F$9/COS(RADIANS(0))*P32)+(1/COS(RADIANS(15))*R32))</f>
-        <v>104.47600639594387</v>
-      </c>
-      <c r="T32" s="152">
+        <v>103.98772071014974</v>
+      </c>
+      <c r="T32" s="147">
         <f>N32*10^3/S32</f>
-        <v>1823.1937319475787</v>
-      </c>
-      <c r="U32" s="153"/>
-      <c r="V32" s="154">
+        <v>1831.7547369937513</v>
+      </c>
+      <c r="U32" s="148"/>
+      <c r="V32" s="149">
         <f>($T$34-T32)^2</f>
-        <v>51938.052878327049</v>
+        <v>52426.959632797596</v>
       </c>
     </row>
     <row r="33" spans="11:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K33" s="162" t="s">
+      <c r="K33" s="157" t="s">
         <v>69</v>
       </c>
-      <c r="L33" s="163">
+      <c r="L33" s="158">
         <v>808</v>
       </c>
-      <c r="M33" s="164">
+      <c r="M33" s="159">
         <v>708</v>
       </c>
-      <c r="N33" s="165">
+      <c r="N33" s="160">
         <f>(L33-M33)*2.381</f>
         <v>238.09999999999997</v>
       </c>
-      <c r="O33" s="166">
+      <c r="O33" s="161">
+        <v>45.37</v>
+      </c>
+      <c r="P33" s="159">
+        <f>O33*$B$2/10</f>
+        <v>51.313469999999995</v>
+      </c>
+      <c r="Q33" s="161">
         <v>45.81</v>
       </c>
-      <c r="P33" s="164">
-        <f>O33*$B$2/10</f>
-        <v>51.811110000000006</v>
-      </c>
-      <c r="Q33" s="166">
-        <v>45.81</v>
-      </c>
-      <c r="R33" s="164">
+      <c r="R33" s="159">
         <f>Q33*$B$2/10</f>
         <v>51.811110000000006</v>
       </c>
-      <c r="S33" s="151">
+      <c r="S33" s="146">
         <f t="shared" si="39"/>
-        <v>104.47600639594387</v>
-      </c>
-      <c r="T33" s="170">
+        <v>103.98772071014974</v>
+      </c>
+      <c r="T33" s="165">
         <f>N33*10^3/S33</f>
-        <v>2278.9921649344728</v>
-      </c>
-      <c r="U33" s="153"/>
-      <c r="V33" s="154">
+        <v>2289.6934212421888</v>
+      </c>
+      <c r="U33" s="148"/>
+      <c r="V33" s="149">
         <f>($T$34-T33)^2</f>
-        <v>51938.052878327049</v>
+        <v>52426.959632797494</v>
       </c>
     </row>
     <row r="34" spans="11:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K34" s="183"/>
-      <c r="L34" s="184"/>
-      <c r="M34" s="184"/>
-      <c r="N34" s="184"/>
-      <c r="O34" s="184"/>
-      <c r="P34" s="184"/>
-      <c r="Q34" s="184"/>
-      <c r="R34" s="184"/>
-      <c r="S34" s="184"/>
-      <c r="T34" s="179">
+      <c r="K34" s="178"/>
+      <c r="L34" s="179"/>
+      <c r="M34" s="179"/>
+      <c r="N34" s="179"/>
+      <c r="O34" s="179"/>
+      <c r="P34" s="179"/>
+      <c r="Q34" s="179"/>
+      <c r="R34" s="179"/>
+      <c r="S34" s="179"/>
+      <c r="T34" s="174">
         <f>SUM(T32:T33)/2</f>
-        <v>2051.0929484410258</v>
-      </c>
-      <c r="U34" s="174" t="s">
+        <v>2060.7240791179702</v>
+      </c>
+      <c r="U34" s="169" t="s">
         <v>48</v>
       </c>
-      <c r="V34" s="180">
+      <c r="V34" s="175">
         <f>SQRT(SUM(V32:V33))</f>
-        <v>322.29816281923496</v>
+        <v>323.8115489997154</v>
       </c>
     </row>
     <row r="35" spans="11:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K35" s="172"/>
-      <c r="L35" s="153"/>
-      <c r="M35" s="153"/>
-      <c r="N35" s="153"/>
-      <c r="O35" s="153"/>
-      <c r="P35" s="153"/>
-      <c r="Q35" s="153"/>
-      <c r="R35" s="153"/>
-      <c r="S35" s="153"/>
-      <c r="T35" s="153"/>
-      <c r="U35" s="153"/>
-      <c r="V35" s="156"/>
+      <c r="K35" s="167"/>
+      <c r="L35" s="148"/>
+      <c r="M35" s="148"/>
+      <c r="N35" s="148"/>
+      <c r="O35" s="148"/>
+      <c r="P35" s="148"/>
+      <c r="Q35" s="148"/>
+      <c r="R35" s="148"/>
+      <c r="S35" s="148"/>
+      <c r="T35" s="148"/>
+      <c r="U35" s="148"/>
+      <c r="V35" s="151"/>
     </row>
     <row r="36" spans="11:48" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K36" s="132" t="s">
+      <c r="K36" s="127" t="s">
         <v>67</v>
       </c>
-      <c r="L36" s="133" t="s">
+      <c r="L36" s="128" t="s">
         <v>54</v>
       </c>
-      <c r="M36" s="134" t="s">
+      <c r="M36" s="129" t="s">
         <v>55</v>
       </c>
-      <c r="N36" s="135" t="s">
+      <c r="N36" s="130" t="s">
         <v>56</v>
       </c>
-      <c r="O36" s="134" t="s">
+      <c r="O36" s="129" t="s">
         <v>57</v>
       </c>
-      <c r="P36" s="135" t="s">
+      <c r="P36" s="130" t="s">
         <v>58</v>
       </c>
-      <c r="Q36" s="134" t="s">
+      <c r="Q36" s="129" t="s">
         <v>59</v>
       </c>
-      <c r="R36" s="135" t="s">
+      <c r="R36" s="130" t="s">
         <v>60</v>
       </c>
-      <c r="S36" s="136" t="s">
+      <c r="S36" s="131" t="s">
         <v>61</v>
       </c>
-      <c r="T36" s="137" t="s">
+      <c r="T36" s="132" t="s">
         <v>62</v>
       </c>
-      <c r="U36" s="153"/>
-      <c r="V36" s="156"/>
+      <c r="U36" s="148"/>
+      <c r="V36" s="151"/>
     </row>
     <row r="37" spans="11:48" x14ac:dyDescent="0.35">
-      <c r="K37" s="145" t="s">
+      <c r="K37" s="140" t="s">
         <v>83</v>
       </c>
-      <c r="L37" s="181">
+      <c r="L37" s="176">
         <v>807</v>
       </c>
-      <c r="M37" s="147">
+      <c r="M37" s="142">
         <v>711</v>
       </c>
-      <c r="N37" s="148">
+      <c r="N37" s="143">
         <f>(L37-M37)*2.381</f>
         <v>228.57599999999996</v>
       </c>
-      <c r="O37" s="147">
+      <c r="O37" s="142">
+        <v>45.37</v>
+      </c>
+      <c r="P37" s="142">
+        <f>O37*$B$2/10</f>
+        <v>51.313469999999995</v>
+      </c>
+      <c r="Q37" s="142">
         <v>45.81</v>
       </c>
-      <c r="P37" s="147">
-        <f>O37*$B$2/10</f>
-        <v>51.811110000000006</v>
-      </c>
-      <c r="Q37" s="147">
-        <v>45.81</v>
-      </c>
-      <c r="R37" s="147">
+      <c r="R37" s="142">
         <f>Q37*$B$2/10</f>
         <v>51.811110000000006</v>
       </c>
-      <c r="S37" s="151">
+      <c r="S37" s="146">
         <f t="shared" ref="S37:S38" si="40">(($F$9/COS(RADIANS(0))*P37)+(1/COS(RADIANS(15))*R37))</f>
-        <v>104.47600639594387</v>
-      </c>
-      <c r="T37" s="152">
+        <v>103.98772071014974</v>
+      </c>
+      <c r="T37" s="147">
         <f>N37*10^3/S37</f>
-        <v>2187.832478337094</v>
-      </c>
-      <c r="U37" s="153"/>
-      <c r="V37" s="154">
+        <v>2198.1056843925012</v>
+      </c>
+      <c r="U37" s="148"/>
+      <c r="V37" s="149">
         <f>($T$23-T37)^2</f>
-        <v>1486596.9185099187</v>
+        <v>1500590.6520897488</v>
       </c>
     </row>
     <row r="38" spans="11:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K38" s="162" t="s">
+      <c r="K38" s="157" t="s">
         <v>87</v>
       </c>
-      <c r="L38" s="163">
+      <c r="L38" s="158">
         <v>808</v>
       </c>
-      <c r="M38" s="164">
+      <c r="M38" s="159">
         <v>720</v>
       </c>
-      <c r="N38" s="165">
+      <c r="N38" s="160">
         <f>(L38-M38)*2.381</f>
         <v>209.52799999999999</v>
       </c>
-      <c r="O38" s="166">
+      <c r="O38" s="161">
+        <v>45.37</v>
+      </c>
+      <c r="P38" s="159">
+        <f>O38*$B$2/10</f>
+        <v>51.313469999999995</v>
+      </c>
+      <c r="Q38" s="161">
         <v>45.81</v>
       </c>
-      <c r="P38" s="164">
-        <f>O38*$B$2/10</f>
-        <v>51.811110000000006</v>
-      </c>
-      <c r="Q38" s="166">
-        <v>45.81</v>
-      </c>
-      <c r="R38" s="164">
+      <c r="R38" s="159">
         <f>Q38*$B$2/10</f>
         <v>51.811110000000006</v>
       </c>
-      <c r="S38" s="151">
+      <c r="S38" s="146">
         <f t="shared" si="40"/>
-        <v>104.47600639594387</v>
-      </c>
-      <c r="T38" s="170">
+        <v>103.98772071014974</v>
+      </c>
+      <c r="T38" s="165">
         <f>N38*10^3/S38</f>
-        <v>2005.5131051423366</v>
-      </c>
-      <c r="U38" s="153"/>
-      <c r="V38" s="154">
+        <v>2014.9302106931264</v>
+      </c>
+      <c r="U38" s="148"/>
+      <c r="V38" s="149">
         <f>($T$23-T38)^2</f>
-        <v>1075247.5397135685</v>
+        <v>1085369.1317979924</v>
       </c>
     </row>
     <row r="39" spans="11:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K39" s="183"/>
-      <c r="L39" s="184"/>
-      <c r="M39" s="184"/>
-      <c r="N39" s="184"/>
-      <c r="O39" s="184"/>
-      <c r="P39" s="184"/>
-      <c r="Q39" s="184"/>
-      <c r="R39" s="184"/>
-      <c r="S39" s="184"/>
-      <c r="T39" s="179">
+      <c r="K39" s="178"/>
+      <c r="L39" s="179"/>
+      <c r="M39" s="179"/>
+      <c r="N39" s="179"/>
+      <c r="O39" s="179"/>
+      <c r="P39" s="179"/>
+      <c r="Q39" s="179"/>
+      <c r="R39" s="179"/>
+      <c r="S39" s="179"/>
+      <c r="T39" s="174">
         <f>SUM(T37:T38)/2</f>
-        <v>2096.6727917397152</v>
-      </c>
-      <c r="U39" s="174" t="s">
+        <v>2106.517947542814</v>
+      </c>
+      <c r="U39" s="169" t="s">
         <v>48</v>
       </c>
-      <c r="V39" s="180">
+      <c r="V39" s="175">
         <f>SQRT(SUM(V37:V38))</f>
-        <v>1600.5762894106258</v>
+        <v>1608.0919699717865</v>
       </c>
     </row>
     <row r="41" spans="11:48" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="42" spans="11:48" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K42" s="132" t="s">
+      <c r="K42" s="127" t="s">
         <v>84</v>
       </c>
-      <c r="L42" s="133" t="s">
+      <c r="L42" s="128" t="s">
         <v>54</v>
       </c>
-      <c r="M42" s="134" t="s">
+      <c r="M42" s="129" t="s">
         <v>55</v>
       </c>
-      <c r="N42" s="135" t="s">
+      <c r="N42" s="130" t="s">
         <v>56</v>
       </c>
-      <c r="O42" s="134" t="s">
+      <c r="O42" s="129" t="s">
         <v>57</v>
       </c>
-      <c r="P42" s="135" t="s">
+      <c r="P42" s="130" t="s">
         <v>58</v>
       </c>
-      <c r="Q42" s="134" t="s">
+      <c r="Q42" s="129" t="s">
         <v>59</v>
       </c>
-      <c r="R42" s="135" t="s">
+      <c r="R42" s="130" t="s">
         <v>60</v>
       </c>
-      <c r="S42" s="136" t="s">
+      <c r="S42" s="131" t="s">
         <v>61</v>
       </c>
-      <c r="T42" s="137" t="s">
+      <c r="T42" s="132" t="s">
         <v>62</v>
       </c>
-      <c r="U42" s="138"/>
-      <c r="V42" s="139"/>
-      <c r="X42" s="186"/>
-      <c r="Y42" s="187" t="s">
+      <c r="U42" s="133"/>
+      <c r="V42" s="134"/>
+      <c r="X42" s="181"/>
+      <c r="Y42" s="182" t="s">
         <v>65</v>
       </c>
-      <c r="Z42" s="188" t="s">
+      <c r="Z42" s="183" t="s">
         <v>66</v>
       </c>
-      <c r="AA42" s="188" t="s">
+      <c r="AA42" s="183" t="s">
         <v>56</v>
       </c>
-      <c r="AB42" s="188" t="s">
+      <c r="AB42" s="183" t="s">
         <v>57</v>
       </c>
-      <c r="AC42" s="188" t="s">
+      <c r="AC42" s="183" t="s">
         <v>58</v>
       </c>
-      <c r="AD42" s="188" t="s">
+      <c r="AD42" s="183" t="s">
         <v>59</v>
       </c>
-      <c r="AE42" s="188" t="s">
+      <c r="AE42" s="183" t="s">
         <v>60</v>
       </c>
-      <c r="AF42" s="189" t="s">
+      <c r="AF42" s="184" t="s">
         <v>61</v>
       </c>
-      <c r="AG42" s="190" t="s">
+      <c r="AG42" s="185" t="s">
         <v>62</v>
       </c>
-      <c r="AH42" s="138"/>
-      <c r="AI42" s="139"/>
-      <c r="AK42" s="140"/>
-      <c r="AL42" s="141" t="s">
+      <c r="AH42" s="133"/>
+      <c r="AI42" s="134"/>
+      <c r="AK42" s="135"/>
+      <c r="AL42" s="136" t="s">
         <v>63</v>
       </c>
-      <c r="AM42" s="142" t="s">
+      <c r="AM42" s="137" t="s">
         <v>64</v>
       </c>
-      <c r="AN42" s="142" t="s">
+      <c r="AN42" s="137" t="s">
         <v>56</v>
       </c>
-      <c r="AO42" s="142" t="s">
+      <c r="AO42" s="137" t="s">
         <v>57</v>
       </c>
-      <c r="AP42" s="142" t="s">
+      <c r="AP42" s="137" t="s">
         <v>58</v>
       </c>
-      <c r="AQ42" s="142" t="s">
+      <c r="AQ42" s="137" t="s">
         <v>59</v>
       </c>
-      <c r="AR42" s="142" t="s">
+      <c r="AR42" s="137" t="s">
         <v>60</v>
       </c>
-      <c r="AS42" s="143" t="s">
+      <c r="AS42" s="138" t="s">
         <v>61</v>
       </c>
-      <c r="AT42" s="201" t="s">
+      <c r="AT42" s="196" t="s">
         <v>62</v>
       </c>
-      <c r="AU42" s="138"/>
-      <c r="AV42" s="139"/>
+      <c r="AU42" s="133"/>
+      <c r="AV42" s="134"/>
     </row>
     <row r="43" spans="11:48" x14ac:dyDescent="0.35">
-      <c r="K43" s="145" t="s">
+      <c r="K43" s="140" t="s">
         <v>82</v>
       </c>
-      <c r="L43" s="181">
+      <c r="L43" s="176">
         <v>806</v>
       </c>
-      <c r="M43" s="147">
+      <c r="M43" s="142">
         <v>775</v>
       </c>
-      <c r="N43" s="148">
-        <f>(L43-M43)*2.381</f>
-        <v>73.810999999999993</v>
-      </c>
-      <c r="O43" s="147">
+      <c r="N43" s="143">
+        <f>(L43-M43)*2.367</f>
+        <v>73.376999999999995</v>
+      </c>
+      <c r="O43" s="142">
+        <v>45.37</v>
+      </c>
+      <c r="P43" s="142">
+        <f>O43*$B$2/10</f>
+        <v>51.313469999999995</v>
+      </c>
+      <c r="Q43" s="142">
         <v>45.81</v>
       </c>
-      <c r="P43" s="147">
-        <f>O43*$B$2/10</f>
-        <v>51.811110000000006</v>
-      </c>
-      <c r="Q43" s="147">
-        <v>45.81</v>
-      </c>
-      <c r="R43" s="147">
+      <c r="R43" s="142">
         <f>Q43*$B$2/10</f>
         <v>51.811110000000006</v>
       </c>
-      <c r="S43" s="151">
+      <c r="S43" s="146">
         <f>(($F$9/COS(RADIANS(0))*P43)+(1/COS(RADIANS(15))*R43))</f>
-        <v>104.47600639594387</v>
-      </c>
-      <c r="T43" s="152">
+        <v>103.98772071014974</v>
+      </c>
+      <c r="T43" s="147">
         <f>N43*10^3/S43</f>
-        <v>706.48757112968667</v>
-      </c>
-      <c r="U43" s="153"/>
-      <c r="V43" s="154">
+        <v>705.63139088823232</v>
+      </c>
+      <c r="U43" s="148"/>
+      <c r="V43" s="149">
         <f>($T$46-T43)^2</f>
-        <v>923.34316228137675</v>
-      </c>
-      <c r="X43" s="191"/>
-      <c r="Y43" s="211">
+        <v>849.37619649661622</v>
+      </c>
+      <c r="X43" s="186"/>
+      <c r="Y43" s="206">
         <v>641</v>
       </c>
-      <c r="Z43" s="210"/>
-      <c r="AA43" s="148">
+      <c r="Z43" s="205"/>
+      <c r="AA43" s="143">
         <f>(AL43-AM43)*2.381</f>
         <v>1402.4089999999999</v>
       </c>
-      <c r="AB43" s="147">
+      <c r="AB43" s="142">
         <v>133.5</v>
       </c>
-      <c r="AC43" s="147">
+      <c r="AC43" s="142">
         <f>AB43*$B$2/10</f>
         <v>150.98849999999999</v>
       </c>
-      <c r="AD43" s="147">
+      <c r="AD43" s="142">
         <v>135.30000000000001</v>
       </c>
-      <c r="AE43" s="147">
+      <c r="AE43" s="142">
         <f>AD43*$B$2/10</f>
         <v>153.02430000000001</v>
       </c>
-      <c r="AF43" s="151">
+      <c r="AF43" s="146">
         <f>(($F$9/COS(RADIANS(0))*AC43)+(1/COS(RADIANS(15)*AE43)))</f>
         <v>146.74501411526421</v>
       </c>
-      <c r="AG43" s="197">
+      <c r="AG43" s="192">
         <f>AA43*10^3/AF43</f>
         <v>9556.7744393580942</v>
       </c>
-      <c r="AH43" s="153"/>
-      <c r="AI43" s="156"/>
-      <c r="AK43" s="155"/>
-      <c r="AL43" s="182">
+      <c r="AH43" s="148"/>
+      <c r="AI43" s="151"/>
+      <c r="AK43" s="150"/>
+      <c r="AL43" s="177">
         <v>589</v>
       </c>
-      <c r="AM43" s="147"/>
-      <c r="AN43" s="148" t="e">
+      <c r="AM43" s="142"/>
+      <c r="AN43" s="143" t="e">
         <f>(#REF!-#REF!)*2.381</f>
         <v>#REF!</v>
       </c>
-      <c r="AO43" s="147">
+      <c r="AO43" s="142">
         <v>139.5</v>
       </c>
-      <c r="AP43" s="147">
+      <c r="AP43" s="142">
         <f>AO43*$B$2/10</f>
         <v>157.77450000000002</v>
       </c>
-      <c r="AQ43" s="147">
+      <c r="AQ43" s="142">
         <v>141.5</v>
       </c>
-      <c r="AR43" s="147">
+      <c r="AR43" s="142">
         <f>AQ43*$B$2/10</f>
         <v>160.03649999999999</v>
       </c>
-      <c r="AS43" s="151">
+      <c r="AS43" s="146">
         <f>(($F$9/COS(RADIANS(0))*AP43)+(1/COS(RADIANS(15)*AR43)))</f>
         <v>152.7750043830697</v>
       </c>
-      <c r="AT43" s="197" t="e">
+      <c r="AT43" s="192" t="e">
         <f>AN43*10^3/AS43</f>
         <v>#REF!</v>
       </c>
-      <c r="AU43" s="153"/>
-      <c r="AV43" s="156"/>
+      <c r="AU43" s="148"/>
+      <c r="AV43" s="151"/>
     </row>
     <row r="44" spans="11:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K44" s="162" t="s">
+      <c r="K44" s="157" t="s">
         <v>69</v>
       </c>
-      <c r="L44" s="163">
+      <c r="L44" s="158">
         <v>806</v>
       </c>
-      <c r="M44" s="164">
+      <c r="M44" s="159">
         <v>774</v>
       </c>
-      <c r="N44" s="165">
-        <f>(L44-M44)*2.381</f>
-        <v>76.191999999999993</v>
-      </c>
-      <c r="O44" s="166">
+      <c r="N44" s="143">
+        <f t="shared" ref="N44:N45" si="41">(L44-M44)*2.367</f>
+        <v>75.744</v>
+      </c>
+      <c r="O44" s="161">
+        <v>45.37</v>
+      </c>
+      <c r="P44" s="159">
+        <f>O44*$B$2/10</f>
+        <v>51.313469999999995</v>
+      </c>
+      <c r="Q44" s="161">
         <v>45.81</v>
       </c>
-      <c r="P44" s="164">
-        <f>O44*$B$2/10</f>
-        <v>51.811110000000006</v>
-      </c>
-      <c r="Q44" s="166">
-        <v>45.81</v>
-      </c>
-      <c r="R44" s="164">
+      <c r="R44" s="159">
         <f>Q44*$B$2/10</f>
         <v>51.811110000000006</v>
       </c>
-      <c r="S44" s="151">
+      <c r="S44" s="146">
         <f>(($F$9/COS(RADIANS(0))*P44)+(1/COS(RADIANS(15))*R44))</f>
-        <v>104.47600639594387</v>
-      </c>
-      <c r="T44" s="170">
+        <v>103.98772071014974</v>
+      </c>
+      <c r="T44" s="165">
         <f>N44*10^3/S44</f>
-        <v>729.27749277903149</v>
-      </c>
-      <c r="U44" s="153"/>
-      <c r="V44" s="154">
+        <v>728.39369382011068</v>
+      </c>
+      <c r="U44" s="148"/>
+      <c r="V44" s="149">
         <f>($T$46-T44)^2</f>
-        <v>57.708947642585613</v>
-      </c>
-      <c r="X44" s="193"/>
-      <c r="Y44" s="163"/>
-      <c r="Z44" s="164"/>
-      <c r="AA44" s="165">
-        <f t="shared" ref="AA44" si="41">(Y44-Z44)*2.381</f>
+        <v>40.726815221171073</v>
+      </c>
+      <c r="X44" s="188"/>
+      <c r="Y44" s="158"/>
+      <c r="Z44" s="159"/>
+      <c r="AA44" s="160">
+        <f t="shared" ref="AA44" si="42">(Y44-Z44)*2.381</f>
         <v>0</v>
       </c>
-      <c r="AB44" s="166">
+      <c r="AB44" s="161">
         <v>133.5</v>
       </c>
-      <c r="AC44" s="164">
-        <f t="shared" ref="AC44" si="42">AB44*$B$2/10</f>
+      <c r="AC44" s="159">
+        <f t="shared" ref="AC44" si="43">AB44*$B$2/10</f>
         <v>150.98849999999999</v>
       </c>
-      <c r="AD44" s="166">
+      <c r="AD44" s="161">
         <v>135.30000000000001</v>
       </c>
-      <c r="AE44" s="164">
-        <f t="shared" ref="AE44" si="43">AD44*$B$2/10</f>
+      <c r="AE44" s="159">
+        <f t="shared" ref="AE44" si="44">AD44*$B$2/10</f>
         <v>153.02430000000001</v>
       </c>
-      <c r="AF44" s="169">
+      <c r="AF44" s="164">
         <f>(($F$9/COS(RADIANS(0))*AC44)+(1/COS(RADIANS(15)*AE44)))</f>
         <v>146.74501411526421</v>
       </c>
-      <c r="AG44" s="199">
+      <c r="AG44" s="194">
         <f>AA44*10^3/AF44</f>
         <v>0</v>
       </c>
-      <c r="AH44" s="153"/>
-      <c r="AI44" s="156"/>
-      <c r="AK44" s="171"/>
-      <c r="AL44" s="177"/>
-      <c r="AM44" s="178"/>
-      <c r="AN44" s="165">
-        <f t="shared" ref="AN44" si="44">(AL44-AM44)*2.381</f>
+      <c r="AH44" s="148"/>
+      <c r="AI44" s="151"/>
+      <c r="AK44" s="166"/>
+      <c r="AL44" s="172"/>
+      <c r="AM44" s="173"/>
+      <c r="AN44" s="160">
+        <f t="shared" ref="AN44" si="45">(AL44-AM44)*2.381</f>
         <v>0</v>
       </c>
-      <c r="AO44" s="166">
+      <c r="AO44" s="161">
         <v>139.5</v>
       </c>
-      <c r="AP44" s="164">
-        <f t="shared" ref="AP44" si="45">AO44*$B$2/10</f>
+      <c r="AP44" s="159">
+        <f t="shared" ref="AP44" si="46">AO44*$B$2/10</f>
         <v>157.77450000000002</v>
       </c>
-      <c r="AQ44" s="166">
+      <c r="AQ44" s="161">
         <v>141.5</v>
       </c>
-      <c r="AR44" s="164">
-        <f t="shared" ref="AR44" si="46">AQ44*$B$2/10</f>
+      <c r="AR44" s="159">
+        <f t="shared" ref="AR44" si="47">AQ44*$B$2/10</f>
         <v>160.03649999999999</v>
       </c>
-      <c r="AS44" s="169">
+      <c r="AS44" s="164">
         <f>(($F$9/COS(RADIANS(0))*AP44)+(1/COS(RADIANS(15)*AR44)))</f>
         <v>152.7750043830697</v>
       </c>
-      <c r="AT44" s="199">
+      <c r="AT44" s="194">
         <f>AN44*10^3/AS44</f>
         <v>0</v>
       </c>
-      <c r="AU44" s="153"/>
-      <c r="AV44" s="156"/>
+      <c r="AU44" s="148"/>
+      <c r="AV44" s="151"/>
     </row>
     <row r="45" spans="11:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K45" s="162" t="s">
+      <c r="K45" s="157" t="s">
         <v>85</v>
       </c>
-      <c r="L45" s="163">
+      <c r="L45" s="158">
         <v>806</v>
       </c>
-      <c r="M45" s="164">
+      <c r="M45" s="159">
         <v>772</v>
       </c>
-      <c r="N45" s="165">
-        <f>(L45-M45)*2.381</f>
-        <v>80.953999999999994</v>
-      </c>
-      <c r="O45" s="166">
+      <c r="N45" s="143">
+        <f t="shared" si="41"/>
+        <v>80.477999999999994</v>
+      </c>
+      <c r="O45" s="161">
         <v>45.81</v>
       </c>
-      <c r="P45" s="164">
+      <c r="P45" s="159">
         <f>O45*$B$2/10</f>
         <v>51.811110000000006</v>
       </c>
-      <c r="Q45" s="166">
+      <c r="Q45" s="161">
         <v>45.81</v>
       </c>
-      <c r="R45" s="164">
+      <c r="R45" s="159">
         <f>Q45*$B$2/10</f>
         <v>51.811110000000006</v>
       </c>
-      <c r="S45" s="151">
+      <c r="S45" s="146">
         <f>(($F$9/COS(RADIANS(0))*P45)+(1/COS(RADIANS(15))*R45))</f>
         <v>104.47600639594387</v>
       </c>
-      <c r="T45" s="170">
+      <c r="T45" s="165">
         <f>N45*10^3/S45</f>
-        <v>774.8573360777209</v>
-      </c>
-      <c r="U45" s="153"/>
-      <c r="V45" s="154">
+        <v>770.30126606298427</v>
+      </c>
+      <c r="U45" s="148"/>
+      <c r="V45" s="149">
         <f>($T$46-T45)^2</f>
-        <v>1442.7236910646402</v>
-      </c>
-      <c r="X45" s="183"/>
-      <c r="Y45" s="184"/>
-      <c r="Z45" s="184"/>
-      <c r="AA45" s="184"/>
-      <c r="AB45" s="184"/>
-      <c r="AC45" s="184"/>
-      <c r="AD45" s="184"/>
-      <c r="AE45" s="184"/>
-      <c r="AF45" s="184"/>
-      <c r="AG45" s="184"/>
-      <c r="AH45" s="184"/>
-      <c r="AI45" s="185"/>
-      <c r="AK45" s="183"/>
-      <c r="AL45" s="184"/>
-      <c r="AM45" s="184"/>
-      <c r="AN45" s="184"/>
-      <c r="AO45" s="184"/>
-      <c r="AP45" s="184"/>
-      <c r="AQ45" s="184"/>
-      <c r="AR45" s="184"/>
-      <c r="AS45" s="184"/>
-      <c r="AT45" s="184"/>
-      <c r="AU45" s="184"/>
-      <c r="AV45" s="185"/>
+        <v>1262.0835886729681</v>
+      </c>
+      <c r="X45" s="178"/>
+      <c r="Y45" s="179"/>
+      <c r="Z45" s="179"/>
+      <c r="AA45" s="179"/>
+      <c r="AB45" s="179"/>
+      <c r="AC45" s="179"/>
+      <c r="AD45" s="179"/>
+      <c r="AE45" s="179"/>
+      <c r="AF45" s="179"/>
+      <c r="AG45" s="179"/>
+      <c r="AH45" s="179"/>
+      <c r="AI45" s="180"/>
+      <c r="AK45" s="178"/>
+      <c r="AL45" s="179"/>
+      <c r="AM45" s="179"/>
+      <c r="AN45" s="179"/>
+      <c r="AO45" s="179"/>
+      <c r="AP45" s="179"/>
+      <c r="AQ45" s="179"/>
+      <c r="AR45" s="179"/>
+      <c r="AS45" s="179"/>
+      <c r="AT45" s="179"/>
+      <c r="AU45" s="179"/>
+      <c r="AV45" s="180"/>
     </row>
     <row r="46" spans="11:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K46" s="183"/>
-      <c r="L46" s="184"/>
-      <c r="M46" s="184"/>
-      <c r="N46" s="184"/>
-      <c r="O46" s="184"/>
-      <c r="P46" s="184"/>
-      <c r="Q46" s="184"/>
-      <c r="R46" s="184"/>
-      <c r="S46" s="184"/>
-      <c r="T46" s="179">
+      <c r="K46" s="178"/>
+      <c r="L46" s="179"/>
+      <c r="M46" s="179"/>
+      <c r="N46" s="179"/>
+      <c r="O46" s="179"/>
+      <c r="P46" s="179"/>
+      <c r="Q46" s="179"/>
+      <c r="R46" s="179"/>
+      <c r="S46" s="179"/>
+      <c r="T46" s="174">
         <f>SUM(T43:T45)/3</f>
-        <v>736.87413332881306</v>
-      </c>
-      <c r="U46" s="174" t="s">
+        <v>734.77545025710913</v>
+      </c>
+      <c r="U46" s="169" t="s">
         <v>48</v>
       </c>
-      <c r="V46" s="180">
+      <c r="V46" s="175">
         <f>SQRT(SUM(V43:V44)/2)</f>
-        <v>22.147822804103818</v>
+        <v>21.096243880342623</v>
       </c>
     </row>
     <row r="47" spans="11:48" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="48" spans="11:48" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="X48" s="186" t="s">
+      <c r="X48" s="181" t="s">
         <v>88</v>
       </c>
-      <c r="Y48" s="187" t="s">
+      <c r="Y48" s="182" t="s">
         <v>65</v>
       </c>
-      <c r="Z48" s="188" t="s">
+      <c r="Z48" s="183" t="s">
         <v>66</v>
       </c>
-      <c r="AA48" s="188" t="s">
+      <c r="AA48" s="183" t="s">
         <v>56</v>
       </c>
-      <c r="AB48" s="188" t="s">
+      <c r="AB48" s="183" t="s">
         <v>57</v>
       </c>
-      <c r="AC48" s="188" t="s">
+      <c r="AC48" s="183" t="s">
         <v>58</v>
       </c>
-      <c r="AD48" s="188" t="s">
+      <c r="AD48" s="183" t="s">
         <v>59</v>
       </c>
-      <c r="AE48" s="188" t="s">
+      <c r="AE48" s="183" t="s">
         <v>60</v>
       </c>
-      <c r="AF48" s="189" t="s">
+      <c r="AF48" s="184" t="s">
         <v>61</v>
       </c>
-      <c r="AG48" s="190" t="s">
+      <c r="AG48" s="185" t="s">
         <v>62</v>
       </c>
-      <c r="AH48" s="138"/>
-      <c r="AI48" s="139"/>
-      <c r="AK48" s="140"/>
-      <c r="AL48" s="141" t="s">
+      <c r="AH48" s="133"/>
+      <c r="AI48" s="134"/>
+      <c r="AK48" s="135"/>
+      <c r="AL48" s="136" t="s">
         <v>63</v>
       </c>
-      <c r="AM48" s="142" t="s">
+      <c r="AM48" s="137" t="s">
         <v>64</v>
       </c>
-      <c r="AN48" s="142" t="s">
+      <c r="AN48" s="137" t="s">
         <v>56</v>
       </c>
-      <c r="AO48" s="142" t="s">
+      <c r="AO48" s="137" t="s">
         <v>57</v>
       </c>
-      <c r="AP48" s="142" t="s">
+      <c r="AP48" s="137" t="s">
         <v>58</v>
       </c>
-      <c r="AQ48" s="142" t="s">
+      <c r="AQ48" s="137" t="s">
         <v>59</v>
       </c>
-      <c r="AR48" s="142" t="s">
+      <c r="AR48" s="137" t="s">
         <v>60</v>
       </c>
-      <c r="AS48" s="143" t="s">
+      <c r="AS48" s="138" t="s">
         <v>61</v>
       </c>
-      <c r="AT48" s="201" t="s">
+      <c r="AT48" s="196" t="s">
         <v>62</v>
       </c>
-      <c r="AU48" s="138"/>
-      <c r="AV48" s="139"/>
+      <c r="AU48" s="133"/>
+      <c r="AV48" s="134"/>
     </row>
     <row r="49" spans="24:48" x14ac:dyDescent="0.35">
-      <c r="X49" s="191" t="s">
+      <c r="X49" s="186" t="s">
         <v>76</v>
       </c>
-      <c r="Y49" s="211">
+      <c r="Y49" s="206">
         <v>641</v>
       </c>
-      <c r="Z49" s="210"/>
-      <c r="AA49" s="148">
+      <c r="Z49" s="205"/>
+      <c r="AA49" s="143">
         <f>(AL49-AM49)*2.381</f>
         <v>1402.4089999999999</v>
       </c>
-      <c r="AB49" s="147">
+      <c r="AB49" s="142">
         <v>133.5</v>
       </c>
-      <c r="AC49" s="147">
+      <c r="AC49" s="142">
         <f>AB49*$B$2/10</f>
         <v>150.98849999999999</v>
       </c>
-      <c r="AD49" s="147">
+      <c r="AD49" s="142">
         <v>135.30000000000001</v>
       </c>
-      <c r="AE49" s="147">
+      <c r="AE49" s="142">
         <f>AD49*$B$2/10</f>
         <v>153.02430000000001</v>
       </c>
-      <c r="AF49" s="151">
+      <c r="AF49" s="146">
         <f>(($F$9/COS(RADIANS(0))*AC49)+(1/COS(RADIANS(15)*AE49)))</f>
         <v>146.74501411526421</v>
       </c>
-      <c r="AG49" s="197">
+      <c r="AG49" s="192">
         <f>AA49*10^3/AF49</f>
         <v>9556.7744393580942</v>
       </c>
-      <c r="AH49" s="153"/>
-      <c r="AI49" s="156"/>
-      <c r="AK49" s="155"/>
-      <c r="AL49" s="182">
+      <c r="AH49" s="148"/>
+      <c r="AI49" s="151"/>
+      <c r="AK49" s="150"/>
+      <c r="AL49" s="177">
         <v>589</v>
       </c>
-      <c r="AM49" s="147"/>
-      <c r="AN49" s="148" t="e">
+      <c r="AM49" s="142"/>
+      <c r="AN49" s="143" t="e">
         <f>(#REF!-#REF!)*2.381</f>
         <v>#REF!</v>
       </c>
-      <c r="AO49" s="147">
+      <c r="AO49" s="142">
         <v>139.5</v>
       </c>
-      <c r="AP49" s="147">
+      <c r="AP49" s="142">
         <f>AO49*$B$2/10</f>
         <v>157.77450000000002</v>
       </c>
-      <c r="AQ49" s="147">
+      <c r="AQ49" s="142">
         <v>141.5</v>
       </c>
-      <c r="AR49" s="147">
+      <c r="AR49" s="142">
         <f>AQ49*$B$2/10</f>
         <v>160.03649999999999</v>
       </c>
-      <c r="AS49" s="151">
+      <c r="AS49" s="146">
         <f>(($F$9/COS(RADIANS(0))*AP49)+(1/COS(RADIANS(15)*AR49)))</f>
         <v>152.7750043830697</v>
       </c>
-      <c r="AT49" s="197" t="e">
+      <c r="AT49" s="192" t="e">
         <f>AN49*10^3/AS49</f>
         <v>#REF!</v>
       </c>
-      <c r="AU49" s="153"/>
-      <c r="AV49" s="156"/>
+      <c r="AU49" s="148"/>
+      <c r="AV49" s="151"/>
     </row>
     <row r="50" spans="24:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="X50" s="193" t="s">
+      <c r="X50" s="188" t="s">
         <v>78</v>
       </c>
-      <c r="Y50" s="163">
+      <c r="Y50" s="158">
         <v>641</v>
       </c>
-      <c r="Z50" s="164"/>
-      <c r="AA50" s="165">
-        <f t="shared" ref="AA50" si="47">(Y50-Z50)*2.381</f>
+      <c r="Z50" s="159"/>
+      <c r="AA50" s="160">
+        <f t="shared" ref="AA50" si="48">(Y50-Z50)*2.381</f>
         <v>1526.2209999999998</v>
       </c>
-      <c r="AB50" s="166">
+      <c r="AB50" s="161">
         <v>133.5</v>
       </c>
-      <c r="AC50" s="164">
-        <f t="shared" ref="AC50" si="48">AB50*$B$2/10</f>
+      <c r="AC50" s="159">
+        <f t="shared" ref="AC50" si="49">AB50*$B$2/10</f>
         <v>150.98849999999999</v>
       </c>
-      <c r="AD50" s="166">
+      <c r="AD50" s="161">
         <v>135.30000000000001</v>
       </c>
-      <c r="AE50" s="164">
-        <f t="shared" ref="AE50" si="49">AD50*$B$2/10</f>
+      <c r="AE50" s="159">
+        <f t="shared" ref="AE50" si="50">AD50*$B$2/10</f>
         <v>153.02430000000001</v>
       </c>
-      <c r="AF50" s="169">
+      <c r="AF50" s="164">
         <f>(($F$9/COS(RADIANS(0))*AC50)+(1/COS(RADIANS(15)*AE50)))</f>
         <v>146.74501411526421</v>
       </c>
-      <c r="AG50" s="199">
+      <c r="AG50" s="194">
         <f>AA50*10^3/AF50</f>
         <v>10400.496461168996</v>
       </c>
-      <c r="AH50" s="153"/>
-      <c r="AI50" s="156"/>
-      <c r="AK50" s="171"/>
-      <c r="AL50" s="177">
+      <c r="AH50" s="148"/>
+      <c r="AI50" s="151"/>
+      <c r="AK50" s="166"/>
+      <c r="AL50" s="172">
         <v>589</v>
       </c>
-      <c r="AM50" s="178"/>
-      <c r="AN50" s="165">
-        <f t="shared" ref="AN50" si="50">(AL50-AM50)*2.381</f>
+      <c r="AM50" s="173"/>
+      <c r="AN50" s="160">
+        <f t="shared" ref="AN50" si="51">(AL50-AM50)*2.381</f>
         <v>1402.4089999999999</v>
       </c>
-      <c r="AO50" s="166">
+      <c r="AO50" s="161">
         <v>139.5</v>
       </c>
-      <c r="AP50" s="164">
-        <f t="shared" ref="AP50" si="51">AO50*$B$2/10</f>
+      <c r="AP50" s="159">
+        <f t="shared" ref="AP50" si="52">AO50*$B$2/10</f>
         <v>157.77450000000002</v>
       </c>
-      <c r="AQ50" s="166">
+      <c r="AQ50" s="161">
         <v>141.5</v>
       </c>
-      <c r="AR50" s="164">
-        <f t="shared" ref="AR50" si="52">AQ50*$B$2/10</f>
+      <c r="AR50" s="159">
+        <f t="shared" ref="AR50" si="53">AQ50*$B$2/10</f>
         <v>160.03649999999999</v>
       </c>
-      <c r="AS50" s="169">
+      <c r="AS50" s="164">
         <f>(($F$9/COS(RADIANS(0))*AP50)+(1/COS(RADIANS(15)*AR50)))</f>
         <v>152.7750043830697</v>
       </c>
-      <c r="AT50" s="199">
+      <c r="AT50" s="194">
         <f>AN50*10^3/AS50</f>
         <v>9179.5710015729037</v>
       </c>
-      <c r="AU50" s="153"/>
-      <c r="AV50" s="156"/>
+      <c r="AU50" s="148"/>
+      <c r="AV50" s="151"/>
     </row>
     <row r="51" spans="24:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="X51" s="183"/>
-      <c r="Y51" s="184"/>
-      <c r="Z51" s="184"/>
-      <c r="AA51" s="184"/>
-      <c r="AB51" s="184"/>
-      <c r="AC51" s="184"/>
-      <c r="AD51" s="184"/>
-      <c r="AE51" s="184"/>
-      <c r="AF51" s="184"/>
-      <c r="AG51" s="184"/>
-      <c r="AH51" s="184"/>
-      <c r="AI51" s="185"/>
-      <c r="AK51" s="183"/>
-      <c r="AL51" s="184"/>
-      <c r="AM51" s="184"/>
-      <c r="AN51" s="184"/>
-      <c r="AO51" s="184"/>
-      <c r="AP51" s="184"/>
-      <c r="AQ51" s="184"/>
-      <c r="AR51" s="184"/>
-      <c r="AS51" s="184"/>
-      <c r="AT51" s="184"/>
-      <c r="AU51" s="184"/>
-      <c r="AV51" s="185"/>
+      <c r="X51" s="178"/>
+      <c r="Y51" s="179"/>
+      <c r="Z51" s="179"/>
+      <c r="AA51" s="179"/>
+      <c r="AB51" s="179"/>
+      <c r="AC51" s="179"/>
+      <c r="AD51" s="179"/>
+      <c r="AE51" s="179"/>
+      <c r="AF51" s="179"/>
+      <c r="AG51" s="179"/>
+      <c r="AH51" s="179"/>
+      <c r="AI51" s="180"/>
+      <c r="AK51" s="178"/>
+      <c r="AL51" s="179"/>
+      <c r="AM51" s="179"/>
+      <c r="AN51" s="179"/>
+      <c r="AO51" s="179"/>
+      <c r="AP51" s="179"/>
+      <c r="AQ51" s="179"/>
+      <c r="AR51" s="179"/>
+      <c r="AS51" s="179"/>
+      <c r="AT51" s="179"/>
+      <c r="AU51" s="179"/>
+      <c r="AV51" s="180"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>